<commit_message>
Alterado o nome do grupo ProdPerigosos para ProdutosPerigosos.
</commit_message>
<xml_diff>
--- a/Emissão/Layouts/LAYOUT 3.0 MDFe.xlsx
+++ b/Emissão/Layouts/LAYOUT 3.0 MDFe.xlsx
@@ -2401,7 +2401,7 @@
     <t xml:space="preserve">D27</t>
   </si>
   <si>
-    <t xml:space="preserve">      ProdPerigosos</t>
+    <t xml:space="preserve">      ProdutosPerigosos</t>
   </si>
   <si>
     <t xml:space="preserve">Grupo de Informações dos Produtos Perigosos</t>
@@ -2410,7 +2410,7 @@
     <t xml:space="preserve">D28</t>
   </si>
   <si>
-    <t xml:space="preserve">       ProdPerigososItem</t>
+    <t xml:space="preserve">       ProdutosPerigososItem</t>
   </si>
   <si>
     <t xml:space="preserve">D29</t>
@@ -3470,176 +3470,176 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="112">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3647,287 +3647,275 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4005,19 +3993,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:S363"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B176" activeCellId="0" sqref="B176"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A262" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D267" activeCellId="0" sqref="D267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="28.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="36.84"/>
@@ -4025,9 +4013,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="6.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="74.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="9.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="2" width="9.16"/>
   </cols>
   <sheetData>
@@ -7772,40 +7760,40 @@
       </c>
     </row>
     <row r="103" s="7" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="76" t="n">
+      <c r="A103" s="39" t="n">
         <f aca="false">A102+1</f>
         <v>77</v>
       </c>
-      <c r="B103" s="77" t="str">
+      <c r="B103" s="40" t="str">
         <f aca="false">CONCATENATE("Ca",TEXT(A103-$A$73, "00"))</f>
         <v>Ca27</v>
       </c>
-      <c r="C103" s="78" t="s">
+      <c r="C103" s="41" t="s">
         <v>305</v>
       </c>
-      <c r="D103" s="78" t="s">
+      <c r="D103" s="41" t="s">
         <v>306</v>
       </c>
-      <c r="E103" s="76" t="s">
+      <c r="E103" s="39" t="s">
         <v>23</v>
       </c>
       <c r="F103" s="44" t="str">
         <f aca="false">$B$95</f>
         <v>Ca19</v>
       </c>
-      <c r="G103" s="76" t="s">
+      <c r="G103" s="39" t="s">
         <v>307</v>
       </c>
-      <c r="H103" s="79" t="s">
+      <c r="H103" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I103" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="J103" s="80" t="s">
+      <c r="I103" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J103" s="76" t="s">
         <v>308</v>
       </c>
-      <c r="K103" s="77" t="s">
+      <c r="K103" s="40" t="s">
         <v>309</v>
       </c>
     </row>
@@ -7838,7 +7826,7 @@
       <c r="I104" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="J104" s="81" t="s">
+      <c r="J104" s="77" t="s">
         <v>314</v>
       </c>
       <c r="K104" s="68" t="s">
@@ -7875,7 +7863,7 @@
       <c r="I105" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="J105" s="82"/>
+      <c r="J105" s="78"/>
       <c r="K105" s="63" t="s">
         <v>76</v>
       </c>
@@ -7908,7 +7896,7 @@
       <c r="I106" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J106" s="83" t="s">
+      <c r="J106" s="79" t="s">
         <v>132</v>
       </c>
       <c r="K106" s="45" t="s">
@@ -8052,7 +8040,7 @@
       <c r="I110" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="J110" s="82" t="s">
+      <c r="J110" s="78" t="s">
         <v>331</v>
       </c>
       <c r="K110" s="63" t="s">
@@ -8087,7 +8075,7 @@
       <c r="I111" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J111" s="83" t="s">
+      <c r="J111" s="79" t="s">
         <v>132</v>
       </c>
       <c r="K111" s="45" t="s">
@@ -8095,76 +8083,76 @@
       </c>
     </row>
     <row r="112" s="7" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="76" t="n">
+      <c r="A112" s="39" t="n">
         <f aca="false">A111+1</f>
         <v>85</v>
       </c>
-      <c r="B112" s="77" t="str">
+      <c r="B112" s="40" t="str">
         <f aca="false">CONCATENATE("Ca",TEXT(A112-$A$73, "00"))</f>
         <v>Ca35</v>
       </c>
-      <c r="C112" s="78" t="s">
+      <c r="C112" s="41" t="s">
         <v>334</v>
       </c>
-      <c r="D112" s="78" t="s">
+      <c r="D112" s="41" t="s">
         <v>335</v>
       </c>
-      <c r="E112" s="76" t="s">
-        <v>23</v>
-      </c>
-      <c r="F112" s="76" t="s">
+      <c r="E112" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F112" s="39" t="s">
         <v>336</v>
       </c>
-      <c r="G112" s="76" t="s">
+      <c r="G112" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="H112" s="79" t="s">
+      <c r="H112" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I112" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="J112" s="80" t="s">
+      <c r="I112" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J112" s="76" t="s">
         <v>337</v>
       </c>
-      <c r="K112" s="77" t="s">
+      <c r="K112" s="40" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="113" s="7" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="76" t="n">
+      <c r="A113" s="39" t="n">
         <f aca="false">A112+1</f>
         <v>86</v>
       </c>
-      <c r="B113" s="77" t="str">
+      <c r="B113" s="40" t="str">
         <f aca="false">CONCATENATE("Ca",TEXT(A113-$A$73, "00"))</f>
         <v>Ca36</v>
       </c>
-      <c r="C113" s="78" t="s">
+      <c r="C113" s="41" t="s">
         <v>338</v>
       </c>
-      <c r="D113" s="78" t="s">
+      <c r="D113" s="41" t="s">
         <v>339</v>
       </c>
-      <c r="E113" s="76" t="s">
-        <v>23</v>
-      </c>
-      <c r="F113" s="76" t="s">
+      <c r="E113" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F113" s="39" t="s">
         <v>336</v>
       </c>
-      <c r="G113" s="76" t="s">
+      <c r="G113" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="H113" s="79" t="s">
+      <c r="H113" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I113" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="J113" s="77" t="s">
+      <c r="I113" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J113" s="40" t="s">
         <v>340</v>
       </c>
-      <c r="K113" s="77" t="s">
+      <c r="K113" s="40" t="s">
         <v>309</v>
       </c>
     </row>
@@ -8233,7 +8221,7 @@
       <c r="I115" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="J115" s="82"/>
+      <c r="J115" s="78"/>
       <c r="K115" s="63" t="s">
         <v>76</v>
       </c>
@@ -8268,7 +8256,7 @@
       <c r="I116" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J116" s="84" t="s">
+      <c r="J116" s="80" t="s">
         <v>349</v>
       </c>
       <c r="K116" s="45" t="s">
@@ -8305,7 +8293,7 @@
       <c r="I117" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J117" s="84"/>
+      <c r="J117" s="80"/>
       <c r="K117" s="45" t="s">
         <v>76</v>
       </c>
@@ -8340,7 +8328,7 @@
       <c r="I118" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J118" s="85" t="s">
+      <c r="J118" s="81" t="s">
         <v>354</v>
       </c>
       <c r="K118" s="45" t="s">
@@ -8377,7 +8365,7 @@
       <c r="I119" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J119" s="85" t="s">
+      <c r="J119" s="81" t="s">
         <v>357</v>
       </c>
       <c r="K119" s="45" t="s">
@@ -8410,7 +8398,7 @@
         <v>34</v>
       </c>
       <c r="I120" s="67"/>
-      <c r="J120" s="86" t="s">
+      <c r="J120" s="82" t="s">
         <v>362</v>
       </c>
       <c r="K120" s="68" t="s">
@@ -8877,7 +8865,7 @@
       <c r="I131" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="J131" s="87" t="s">
+      <c r="J131" s="83" t="s">
         <v>396</v>
       </c>
       <c r="K131" s="63" t="s">
@@ -9833,7 +9821,7 @@
       <c r="R152" s="7"/>
       <c r="S152" s="7"/>
     </row>
-    <row r="153" s="88" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" s="84" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="61" t="n">
         <f aca="false">A152+1</f>
         <v>123</v>
@@ -9908,7 +9896,7 @@
       <c r="I154" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="J154" s="89" t="s">
+      <c r="J154" s="85" t="s">
         <v>400</v>
       </c>
       <c r="K154" s="40" t="s">
@@ -9953,7 +9941,7 @@
       <c r="I155" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="J155" s="89"/>
+      <c r="J155" s="85"/>
       <c r="K155" s="40" t="s">
         <v>20</v>
       </c>
@@ -13234,7 +13222,7 @@
       <c r="I239" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J239" s="90" t="s">
+      <c r="J239" s="86" t="s">
         <v>132</v>
       </c>
       <c r="K239" s="45" t="s">
@@ -14235,7 +14223,7 @@
       <c r="R262" s="7"/>
       <c r="S262" s="7"/>
     </row>
-    <row r="263" s="7" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" s="7" customFormat="true" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="61" t="n">
         <f aca="false">A262+1</f>
         <v>221</v>
@@ -14296,7 +14284,7 @@
       <c r="I264" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J264" s="90" t="s">
+      <c r="J264" s="86" t="s">
         <v>132</v>
       </c>
       <c r="K264" s="45" t="s">
@@ -14693,19 +14681,19 @@
       <c r="S275" s="7"/>
     </row>
     <row r="276" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="91" t="s">
+      <c r="A276" s="87" t="s">
         <v>810</v>
       </c>
-      <c r="B276" s="91"/>
-      <c r="C276" s="91"/>
-      <c r="D276" s="91"/>
-      <c r="E276" s="91"/>
-      <c r="F276" s="91"/>
-      <c r="G276" s="91"/>
-      <c r="H276" s="91"/>
-      <c r="I276" s="91"/>
-      <c r="J276" s="91"/>
-      <c r="K276" s="91"/>
+      <c r="B276" s="87"/>
+      <c r="C276" s="87"/>
+      <c r="D276" s="87"/>
+      <c r="E276" s="87"/>
+      <c r="F276" s="87"/>
+      <c r="G276" s="87"/>
+      <c r="H276" s="87"/>
+      <c r="I276" s="87"/>
+      <c r="J276" s="87"/>
+      <c r="K276" s="87"/>
     </row>
     <row r="277" s="7" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="44" t="n">
@@ -15012,7 +15000,7 @@
       <c r="I285" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J285" s="92" t="s">
+      <c r="J285" s="88" t="s">
         <v>164</v>
       </c>
       <c r="K285" s="45" t="s">
@@ -15048,7 +15036,7 @@
       <c r="I286" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J286" s="92"/>
+      <c r="J286" s="88"/>
       <c r="K286" s="45" t="s">
         <v>76</v>
       </c>
@@ -15082,7 +15070,7 @@
       <c r="I287" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="J287" s="82" t="s">
+      <c r="J287" s="78" t="s">
         <v>844</v>
       </c>
       <c r="K287" s="63" t="s">
@@ -15159,16 +15147,16 @@
     </row>
     <row r="290" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="9"/>
-      <c r="B290" s="93"/>
-      <c r="C290" s="94"/>
-      <c r="D290" s="94"/>
+      <c r="B290" s="89"/>
+      <c r="C290" s="90"/>
+      <c r="D290" s="90"/>
       <c r="E290" s="9"/>
       <c r="F290" s="9"/>
       <c r="G290" s="9"/>
-      <c r="H290" s="95"/>
+      <c r="H290" s="91"/>
       <c r="I290" s="9"/>
-      <c r="J290" s="93"/>
-      <c r="K290" s="93"/>
+      <c r="J290" s="89"/>
+      <c r="K290" s="89"/>
     </row>
     <row r="291" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="12" t="s">
@@ -15214,19 +15202,19 @@
       <c r="S291" s="7"/>
     </row>
     <row r="292" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="91" t="s">
+      <c r="A292" s="87" t="s">
         <v>852</v>
       </c>
-      <c r="B292" s="91"/>
-      <c r="C292" s="91"/>
-      <c r="D292" s="91"/>
-      <c r="E292" s="91"/>
-      <c r="F292" s="91"/>
-      <c r="G292" s="91"/>
-      <c r="H292" s="91"/>
-      <c r="I292" s="91"/>
-      <c r="J292" s="91"/>
-      <c r="K292" s="91"/>
+      <c r="B292" s="87"/>
+      <c r="C292" s="87"/>
+      <c r="D292" s="87"/>
+      <c r="E292" s="87"/>
+      <c r="F292" s="87"/>
+      <c r="G292" s="87"/>
+      <c r="H292" s="87"/>
+      <c r="I292" s="87"/>
+      <c r="J292" s="87"/>
+      <c r="K292" s="87"/>
     </row>
     <row r="293" s="7" customFormat="true" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="44" t="n">
@@ -15503,7 +15491,7 @@
       <c r="I300" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J300" s="85" t="s">
+      <c r="J300" s="81" t="s">
         <v>882</v>
       </c>
       <c r="K300" s="45" t="s">
@@ -15539,7 +15527,7 @@
       <c r="I301" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J301" s="96" t="s">
+      <c r="J301" s="92" t="s">
         <v>886</v>
       </c>
       <c r="K301" s="45" t="s">
@@ -15575,7 +15563,7 @@
       <c r="I302" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J302" s="96"/>
+      <c r="J302" s="92"/>
       <c r="K302" s="45" t="s">
         <v>76</v>
       </c>
@@ -15643,7 +15631,7 @@
       <c r="I304" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J304" s="85" t="s">
+      <c r="J304" s="81" t="s">
         <v>896</v>
       </c>
       <c r="K304" s="45" t="s">
@@ -15679,7 +15667,7 @@
       <c r="I305" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J305" s="96" t="s">
+      <c r="J305" s="92" t="s">
         <v>886</v>
       </c>
       <c r="K305" s="45" t="s">
@@ -15715,23 +15703,23 @@
       <c r="I306" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J306" s="96"/>
+      <c r="J306" s="92"/>
       <c r="K306" s="45" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="307" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="9"/>
-      <c r="B307" s="93"/>
-      <c r="C307" s="94"/>
-      <c r="D307" s="94"/>
+      <c r="B307" s="89"/>
+      <c r="C307" s="90"/>
+      <c r="D307" s="90"/>
       <c r="E307" s="9"/>
       <c r="F307" s="9"/>
       <c r="G307" s="9"/>
-      <c r="H307" s="95"/>
+      <c r="H307" s="91"/>
       <c r="I307" s="9"/>
-      <c r="J307" s="93"/>
-      <c r="K307" s="93"/>
+      <c r="J307" s="89"/>
+      <c r="K307" s="89"/>
     </row>
     <row r="308" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="12" t="s">
@@ -16809,19 +16797,19 @@
       <c r="S336" s="7"/>
     </row>
     <row r="337" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="91" t="s">
+      <c r="A337" s="87" t="s">
         <v>969</v>
       </c>
-      <c r="B337" s="91"/>
-      <c r="C337" s="91"/>
-      <c r="D337" s="91"/>
-      <c r="E337" s="91"/>
-      <c r="F337" s="91"/>
-      <c r="G337" s="91"/>
-      <c r="H337" s="91"/>
-      <c r="I337" s="91"/>
-      <c r="J337" s="91"/>
-      <c r="K337" s="91"/>
+      <c r="B337" s="87"/>
+      <c r="C337" s="87"/>
+      <c r="D337" s="87"/>
+      <c r="E337" s="87"/>
+      <c r="F337" s="87"/>
+      <c r="G337" s="87"/>
+      <c r="H337" s="87"/>
+      <c r="I337" s="87"/>
+      <c r="J337" s="87"/>
+      <c r="K337" s="87"/>
       <c r="L337" s="7"/>
       <c r="M337" s="7"/>
       <c r="N337" s="7"/>
@@ -16959,19 +16947,19 @@
       <c r="S340" s="7"/>
     </row>
     <row r="341" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="91" t="s">
+      <c r="A341" s="87" t="s">
         <v>977</v>
       </c>
-      <c r="B341" s="91"/>
-      <c r="C341" s="91"/>
-      <c r="D341" s="91"/>
-      <c r="E341" s="91"/>
-      <c r="F341" s="91"/>
-      <c r="G341" s="91"/>
-      <c r="H341" s="91"/>
-      <c r="I341" s="91"/>
-      <c r="J341" s="91"/>
-      <c r="K341" s="91"/>
+      <c r="B341" s="87"/>
+      <c r="C341" s="87"/>
+      <c r="D341" s="87"/>
+      <c r="E341" s="87"/>
+      <c r="F341" s="87"/>
+      <c r="G341" s="87"/>
+      <c r="H341" s="87"/>
+      <c r="I341" s="87"/>
+      <c r="J341" s="87"/>
+      <c r="K341" s="87"/>
       <c r="L341" s="7"/>
       <c r="M341" s="7"/>
       <c r="N341" s="7"/>
@@ -17280,15 +17268,15 @@
       <c r="S348" s="7"/>
     </row>
     <row r="349" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="97"/>
+      <c r="A349" s="93"/>
       <c r="B349" s="7"/>
-      <c r="C349" s="98"/>
-      <c r="D349" s="98"/>
-      <c r="E349" s="97"/>
-      <c r="F349" s="97"/>
-      <c r="G349" s="97"/>
-      <c r="H349" s="99"/>
-      <c r="I349" s="97"/>
+      <c r="C349" s="94"/>
+      <c r="D349" s="94"/>
+      <c r="E349" s="93"/>
+      <c r="F349" s="93"/>
+      <c r="G349" s="93"/>
+      <c r="H349" s="95"/>
+      <c r="I349" s="93"/>
       <c r="J349" s="7"/>
       <c r="K349" s="7"/>
       <c r="L349" s="7"/>
@@ -17301,15 +17289,15 @@
       <c r="S349" s="7"/>
     </row>
     <row r="350" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="97"/>
+      <c r="A350" s="93"/>
       <c r="B350" s="7"/>
-      <c r="C350" s="98"/>
-      <c r="D350" s="98"/>
-      <c r="E350" s="97"/>
-      <c r="F350" s="97"/>
-      <c r="G350" s="97"/>
-      <c r="H350" s="99"/>
-      <c r="I350" s="97"/>
+      <c r="C350" s="94"/>
+      <c r="D350" s="94"/>
+      <c r="E350" s="93"/>
+      <c r="F350" s="93"/>
+      <c r="G350" s="93"/>
+      <c r="H350" s="95"/>
+      <c r="I350" s="93"/>
       <c r="J350" s="7"/>
       <c r="K350" s="7"/>
       <c r="L350" s="7"/>
@@ -17322,15 +17310,15 @@
       <c r="S350" s="7"/>
     </row>
     <row r="351" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="97"/>
+      <c r="A351" s="93"/>
       <c r="B351" s="7"/>
-      <c r="C351" s="98"/>
-      <c r="D351" s="98"/>
-      <c r="E351" s="97"/>
-      <c r="F351" s="97"/>
-      <c r="G351" s="97"/>
-      <c r="H351" s="99"/>
-      <c r="I351" s="97"/>
+      <c r="C351" s="94"/>
+      <c r="D351" s="94"/>
+      <c r="E351" s="93"/>
+      <c r="F351" s="93"/>
+      <c r="G351" s="93"/>
+      <c r="H351" s="95"/>
+      <c r="I351" s="93"/>
       <c r="J351" s="7"/>
       <c r="K351" s="7"/>
       <c r="L351" s="7"/>
@@ -17343,15 +17331,15 @@
       <c r="S351" s="7"/>
     </row>
     <row r="352" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="97"/>
+      <c r="A352" s="93"/>
       <c r="B352" s="7"/>
-      <c r="C352" s="98"/>
-      <c r="D352" s="98"/>
-      <c r="E352" s="97"/>
-      <c r="F352" s="97"/>
-      <c r="G352" s="97"/>
-      <c r="H352" s="99"/>
-      <c r="I352" s="97"/>
+      <c r="C352" s="94"/>
+      <c r="D352" s="94"/>
+      <c r="E352" s="93"/>
+      <c r="F352" s="93"/>
+      <c r="G352" s="93"/>
+      <c r="H352" s="95"/>
+      <c r="I352" s="93"/>
       <c r="J352" s="7"/>
       <c r="K352" s="7"/>
       <c r="L352" s="7"/>
@@ -17364,15 +17352,15 @@
       <c r="S352" s="7"/>
     </row>
     <row r="353" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="97"/>
+      <c r="A353" s="93"/>
       <c r="B353" s="7"/>
-      <c r="C353" s="98"/>
-      <c r="D353" s="98"/>
-      <c r="E353" s="97"/>
-      <c r="F353" s="97"/>
-      <c r="G353" s="97"/>
-      <c r="H353" s="99"/>
-      <c r="I353" s="97"/>
+      <c r="C353" s="94"/>
+      <c r="D353" s="94"/>
+      <c r="E353" s="93"/>
+      <c r="F353" s="93"/>
+      <c r="G353" s="93"/>
+      <c r="H353" s="95"/>
+      <c r="I353" s="93"/>
       <c r="J353" s="7"/>
       <c r="K353" s="7"/>
       <c r="L353" s="7"/>
@@ -17385,15 +17373,15 @@
       <c r="S353" s="7"/>
     </row>
     <row r="354" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="97"/>
+      <c r="A354" s="93"/>
       <c r="B354" s="7"/>
-      <c r="C354" s="98"/>
-      <c r="D354" s="98"/>
-      <c r="E354" s="97"/>
-      <c r="F354" s="97"/>
-      <c r="G354" s="97"/>
-      <c r="H354" s="99"/>
-      <c r="I354" s="97"/>
+      <c r="C354" s="94"/>
+      <c r="D354" s="94"/>
+      <c r="E354" s="93"/>
+      <c r="F354" s="93"/>
+      <c r="G354" s="93"/>
+      <c r="H354" s="95"/>
+      <c r="I354" s="93"/>
       <c r="J354" s="7"/>
       <c r="K354" s="7"/>
       <c r="L354" s="7"/>
@@ -17406,15 +17394,15 @@
       <c r="S354" s="7"/>
     </row>
     <row r="355" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="97"/>
+      <c r="A355" s="93"/>
       <c r="B355" s="7"/>
-      <c r="C355" s="98"/>
-      <c r="D355" s="98"/>
-      <c r="E355" s="97"/>
-      <c r="F355" s="97"/>
-      <c r="G355" s="97"/>
-      <c r="H355" s="99"/>
-      <c r="I355" s="97"/>
+      <c r="C355" s="94"/>
+      <c r="D355" s="94"/>
+      <c r="E355" s="93"/>
+      <c r="F355" s="93"/>
+      <c r="G355" s="93"/>
+      <c r="H355" s="95"/>
+      <c r="I355" s="93"/>
       <c r="J355" s="7"/>
       <c r="K355" s="7"/>
       <c r="L355" s="7"/>
@@ -17427,15 +17415,15 @@
       <c r="S355" s="7"/>
     </row>
     <row r="356" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="97"/>
+      <c r="A356" s="93"/>
       <c r="B356" s="7"/>
-      <c r="C356" s="98"/>
-      <c r="D356" s="98"/>
-      <c r="E356" s="97"/>
-      <c r="F356" s="97"/>
-      <c r="G356" s="97"/>
-      <c r="H356" s="99"/>
-      <c r="I356" s="97"/>
+      <c r="C356" s="94"/>
+      <c r="D356" s="94"/>
+      <c r="E356" s="93"/>
+      <c r="F356" s="93"/>
+      <c r="G356" s="93"/>
+      <c r="H356" s="95"/>
+      <c r="I356" s="93"/>
       <c r="J356" s="7"/>
       <c r="K356" s="7"/>
       <c r="L356" s="7"/>
@@ -17448,15 +17436,15 @@
       <c r="S356" s="7"/>
     </row>
     <row r="357" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="97"/>
+      <c r="A357" s="93"/>
       <c r="B357" s="7"/>
-      <c r="C357" s="98"/>
-      <c r="D357" s="98"/>
-      <c r="E357" s="97"/>
-      <c r="F357" s="97"/>
-      <c r="G357" s="97"/>
-      <c r="H357" s="99"/>
-      <c r="I357" s="97"/>
+      <c r="C357" s="94"/>
+      <c r="D357" s="94"/>
+      <c r="E357" s="93"/>
+      <c r="F357" s="93"/>
+      <c r="G357" s="93"/>
+      <c r="H357" s="95"/>
+      <c r="I357" s="93"/>
       <c r="J357" s="7"/>
       <c r="K357" s="7"/>
       <c r="L357" s="7"/>
@@ -17469,15 +17457,15 @@
       <c r="S357" s="7"/>
     </row>
     <row r="358" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="97"/>
+      <c r="A358" s="93"/>
       <c r="B358" s="7"/>
-      <c r="C358" s="98"/>
-      <c r="D358" s="98"/>
-      <c r="E358" s="97"/>
-      <c r="F358" s="97"/>
-      <c r="G358" s="97"/>
-      <c r="H358" s="99"/>
-      <c r="I358" s="97"/>
+      <c r="C358" s="94"/>
+      <c r="D358" s="94"/>
+      <c r="E358" s="93"/>
+      <c r="F358" s="93"/>
+      <c r="G358" s="93"/>
+      <c r="H358" s="95"/>
+      <c r="I358" s="93"/>
       <c r="J358" s="7"/>
       <c r="K358" s="7"/>
       <c r="L358" s="7"/>
@@ -17490,15 +17478,15 @@
       <c r="S358" s="7"/>
     </row>
     <row r="359" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="97"/>
+      <c r="A359" s="93"/>
       <c r="B359" s="7"/>
-      <c r="C359" s="98"/>
-      <c r="D359" s="98"/>
-      <c r="E359" s="97"/>
-      <c r="F359" s="97"/>
-      <c r="G359" s="97"/>
-      <c r="H359" s="99"/>
-      <c r="I359" s="97"/>
+      <c r="C359" s="94"/>
+      <c r="D359" s="94"/>
+      <c r="E359" s="93"/>
+      <c r="F359" s="93"/>
+      <c r="G359" s="93"/>
+      <c r="H359" s="95"/>
+      <c r="I359" s="93"/>
       <c r="J359" s="7"/>
       <c r="K359" s="7"/>
       <c r="L359" s="7"/>
@@ -17511,15 +17499,15 @@
       <c r="S359" s="7"/>
     </row>
     <row r="360" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="97"/>
+      <c r="A360" s="93"/>
       <c r="B360" s="7"/>
-      <c r="C360" s="98"/>
-      <c r="D360" s="98"/>
-      <c r="E360" s="97"/>
-      <c r="F360" s="97"/>
-      <c r="G360" s="97"/>
-      <c r="H360" s="99"/>
-      <c r="I360" s="97"/>
+      <c r="C360" s="94"/>
+      <c r="D360" s="94"/>
+      <c r="E360" s="93"/>
+      <c r="F360" s="93"/>
+      <c r="G360" s="93"/>
+      <c r="H360" s="95"/>
+      <c r="I360" s="93"/>
       <c r="J360" s="7"/>
       <c r="K360" s="7"/>
       <c r="L360" s="7"/>
@@ -17532,15 +17520,15 @@
       <c r="S360" s="7"/>
     </row>
     <row r="361" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="97"/>
+      <c r="A361" s="93"/>
       <c r="B361" s="7"/>
-      <c r="C361" s="98"/>
-      <c r="D361" s="98"/>
-      <c r="E361" s="97"/>
-      <c r="F361" s="97"/>
-      <c r="G361" s="97"/>
-      <c r="H361" s="99"/>
-      <c r="I361" s="97"/>
+      <c r="C361" s="94"/>
+      <c r="D361" s="94"/>
+      <c r="E361" s="93"/>
+      <c r="F361" s="93"/>
+      <c r="G361" s="93"/>
+      <c r="H361" s="95"/>
+      <c r="I361" s="93"/>
       <c r="J361" s="7"/>
       <c r="K361" s="7"/>
       <c r="L361" s="7"/>
@@ -17553,15 +17541,15 @@
       <c r="S361" s="7"/>
     </row>
     <row r="362" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="97"/>
+      <c r="A362" s="93"/>
       <c r="B362" s="7"/>
-      <c r="C362" s="98"/>
-      <c r="D362" s="98"/>
-      <c r="E362" s="97"/>
-      <c r="F362" s="97"/>
-      <c r="G362" s="97"/>
-      <c r="H362" s="99"/>
-      <c r="I362" s="97"/>
+      <c r="C362" s="94"/>
+      <c r="D362" s="94"/>
+      <c r="E362" s="93"/>
+      <c r="F362" s="93"/>
+      <c r="G362" s="93"/>
+      <c r="H362" s="95"/>
+      <c r="I362" s="93"/>
       <c r="J362" s="7"/>
       <c r="K362" s="7"/>
       <c r="L362" s="7"/>
@@ -17626,7 +17614,7 @@
     <hyperlink ref="J240" r:id="rId4" display="Consulte nosso artigo para mais informações."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -17636,7 +17624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -17648,11 +17636,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="36.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="96" width="6.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="96" width="17.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="96" width="40.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="96" width="36.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="96" width="7.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17699,28 +17687,28 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
@@ -17758,19 +17746,19 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="98" t="s">
         <v>1003</v>
       </c>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="n">
@@ -17779,7 +17767,7 @@
       <c r="B8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="102" t="s">
+      <c r="C8" s="99" t="s">
         <v>1004</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -17815,7 +17803,7 @@
       <c r="B9" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="103" t="s">
+      <c r="C9" s="100" t="s">
         <v>1006</v>
       </c>
       <c r="D9" s="25" t="s">
@@ -17851,7 +17839,7 @@
       <c r="B10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="102" t="s">
+      <c r="C10" s="99" t="s">
         <v>1008</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -17887,10 +17875,10 @@
       <c r="B11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="101" t="s">
         <v>1010</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="102" t="s">
         <v>1011</v>
       </c>
       <c r="E11" s="24" t="s">
@@ -17899,7 +17887,7 @@
       <c r="F11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="106" t="s">
+      <c r="G11" s="103" t="s">
         <v>997</v>
       </c>
       <c r="H11" s="21" t="s">
@@ -17908,7 +17896,7 @@
       <c r="I11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="105" t="s">
+      <c r="J11" s="102" t="s">
         <v>1011</v>
       </c>
       <c r="K11" s="19" t="s">
@@ -17923,10 +17911,10 @@
       <c r="B12" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="104" t="s">
+      <c r="C12" s="101" t="s">
         <v>1012</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="102" t="s">
         <v>1013</v>
       </c>
       <c r="E12" s="24" t="s">
@@ -17935,7 +17923,7 @@
       <c r="F12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="106" t="s">
+      <c r="G12" s="103" t="s">
         <v>711</v>
       </c>
       <c r="H12" s="21" t="s">
@@ -17944,7 +17932,7 @@
       <c r="I12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="105" t="s">
+      <c r="J12" s="102" t="s">
         <v>1013</v>
       </c>
       <c r="K12" s="19" t="s">
@@ -17959,10 +17947,10 @@
       <c r="B13" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="101" t="s">
         <v>1014</v>
       </c>
-      <c r="D13" s="105" t="s">
+      <c r="D13" s="102" t="s">
         <v>1015</v>
       </c>
       <c r="E13" s="24" t="s">
@@ -17971,7 +17959,7 @@
       <c r="F13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="106" t="s">
+      <c r="G13" s="103" t="s">
         <v>267</v>
       </c>
       <c r="H13" s="21" t="s">
@@ -17980,7 +17968,7 @@
       <c r="I13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="105" t="s">
+      <c r="J13" s="102" t="s">
         <v>1015</v>
       </c>
       <c r="K13" s="19" t="s">
@@ -17995,10 +17983,10 @@
       <c r="B14" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="101" t="s">
         <v>1016</v>
       </c>
-      <c r="D14" s="105" t="s">
+      <c r="D14" s="102" t="s">
         <v>1017</v>
       </c>
       <c r="E14" s="24" t="s">
@@ -18007,7 +17995,7 @@
       <c r="F14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="106" t="s">
+      <c r="G14" s="103" t="s">
         <v>61</v>
       </c>
       <c r="H14" s="21" t="s">
@@ -18016,7 +18004,7 @@
       <c r="I14" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="105" t="s">
+      <c r="J14" s="102" t="s">
         <v>1017</v>
       </c>
       <c r="K14" s="19" t="s">
@@ -18031,10 +18019,10 @@
       <c r="B15" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="101" t="s">
         <v>1018</v>
       </c>
-      <c r="D15" s="105" t="s">
+      <c r="D15" s="102" t="s">
         <v>1019</v>
       </c>
       <c r="E15" s="24" t="s">
@@ -18043,7 +18031,7 @@
       <c r="F15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="106" t="s">
+      <c r="G15" s="103" t="s">
         <v>375</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -18052,7 +18040,7 @@
       <c r="I15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="105" t="s">
+      <c r="J15" s="102" t="s">
         <v>1020</v>
       </c>
       <c r="K15" s="19" t="s">
@@ -18067,10 +18055,10 @@
       <c r="B16" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="101" t="s">
         <v>1021</v>
       </c>
-      <c r="D16" s="105" t="s">
+      <c r="D16" s="102" t="s">
         <v>1022</v>
       </c>
       <c r="E16" s="24" t="s">
@@ -18079,7 +18067,7 @@
       <c r="F16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="106" t="s">
+      <c r="G16" s="103" t="s">
         <v>1023</v>
       </c>
       <c r="H16" s="21" t="s">
@@ -18088,7 +18076,7 @@
       <c r="I16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="105" t="s">
+      <c r="J16" s="102" t="s">
         <v>1024</v>
       </c>
       <c r="K16" s="19" t="s">
@@ -18103,10 +18091,10 @@
       <c r="B17" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="101" t="s">
         <v>1025</v>
       </c>
-      <c r="D17" s="105" t="s">
+      <c r="D17" s="102" t="s">
         <v>1026</v>
       </c>
       <c r="E17" s="24" t="s">
@@ -18115,7 +18103,7 @@
       <c r="F17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="103" t="s">
         <v>1027</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -18124,7 +18112,7 @@
       <c r="I17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="105" t="s">
+      <c r="J17" s="102" t="s">
         <v>1028</v>
       </c>
       <c r="K17" s="19" t="s">
@@ -18139,10 +18127,10 @@
       <c r="B18" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="101" t="s">
         <v>1029</v>
       </c>
-      <c r="D18" s="105" t="s">
+      <c r="D18" s="102" t="s">
         <v>1030</v>
       </c>
       <c r="E18" s="24" t="s">
@@ -18151,7 +18139,7 @@
       <c r="F18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="106" t="s">
+      <c r="G18" s="103" t="s">
         <v>1027</v>
       </c>
       <c r="H18" s="21" t="s">
@@ -18160,7 +18148,7 @@
       <c r="I18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="105" t="s">
+      <c r="J18" s="102" t="s">
         <v>1031</v>
       </c>
       <c r="K18" s="19" t="s">
@@ -18175,10 +18163,10 @@
       <c r="B19" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="104" t="s">
+      <c r="C19" s="101" t="s">
         <v>1032</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="102" t="s">
         <v>1033</v>
       </c>
       <c r="E19" s="24" t="s">
@@ -18187,7 +18175,7 @@
       <c r="F19" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="106" t="s">
+      <c r="G19" s="103" t="s">
         <v>1027</v>
       </c>
       <c r="H19" s="21" t="s">
@@ -18196,7 +18184,7 @@
       <c r="I19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="105" t="s">
+      <c r="J19" s="102" t="s">
         <v>1034</v>
       </c>
       <c r="K19" s="19" t="s">
@@ -18211,10 +18199,10 @@
       <c r="B20" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="104" t="s">
+      <c r="C20" s="101" t="s">
         <v>1035</v>
       </c>
-      <c r="D20" s="105" t="s">
+      <c r="D20" s="102" t="s">
         <v>1036</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -18223,7 +18211,7 @@
       <c r="F20" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="106" t="s">
+      <c r="G20" s="103" t="s">
         <v>1027</v>
       </c>
       <c r="H20" s="21" t="s">
@@ -18232,7 +18220,7 @@
       <c r="I20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="105" t="s">
+      <c r="J20" s="102" t="s">
         <v>1036</v>
       </c>
       <c r="K20" s="19" t="s">
@@ -18247,10 +18235,10 @@
       <c r="B21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="104" t="s">
+      <c r="C21" s="101" t="s">
         <v>1037</v>
       </c>
-      <c r="D21" s="105" t="s">
+      <c r="D21" s="102" t="s">
         <v>1038</v>
       </c>
       <c r="E21" s="24" t="s">
@@ -18259,7 +18247,7 @@
       <c r="F21" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="106" t="s">
+      <c r="G21" s="103" t="s">
         <v>1027</v>
       </c>
       <c r="H21" s="21" t="s">
@@ -18268,7 +18256,7 @@
       <c r="I21" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="105" t="s">
+      <c r="J21" s="102" t="s">
         <v>1038</v>
       </c>
       <c r="K21" s="19" t="s">
@@ -18283,10 +18271,10 @@
       <c r="B22" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="104" t="s">
+      <c r="C22" s="101" t="s">
         <v>1039</v>
       </c>
-      <c r="D22" s="105" t="s">
+      <c r="D22" s="102" t="s">
         <v>1040</v>
       </c>
       <c r="E22" s="24" t="s">
@@ -18295,7 +18283,7 @@
       <c r="F22" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="106" t="s">
+      <c r="G22" s="103" t="s">
         <v>1041</v>
       </c>
       <c r="H22" s="21" t="s">
@@ -18304,7 +18292,7 @@
       <c r="I22" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="105" t="s">
+      <c r="J22" s="102" t="s">
         <v>1042</v>
       </c>
       <c r="K22" s="19" t="s">
@@ -18316,13 +18304,13 @@
         <f aca="false">A22+1</f>
         <v>16</v>
       </c>
-      <c r="B23" s="107" t="s">
+      <c r="B23" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="104" t="s">
+      <c r="C23" s="101" t="s">
         <v>1043</v>
       </c>
-      <c r="D23" s="105" t="s">
+      <c r="D23" s="102" t="s">
         <v>1044</v>
       </c>
       <c r="E23" s="18" t="s">
@@ -18331,7 +18319,7 @@
       <c r="F23" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="106" t="s">
+      <c r="G23" s="103" t="s">
         <v>17</v>
       </c>
       <c r="H23" s="21" t="s">
@@ -18340,7 +18328,7 @@
       <c r="I23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="105" t="s">
+      <c r="J23" s="102" t="s">
         <v>1044</v>
       </c>
       <c r="K23" s="19" t="s">
@@ -18352,22 +18340,22 @@
         <f aca="false">A23+1</f>
         <v>17</v>
       </c>
-      <c r="B24" s="107" t="s">
+      <c r="B24" s="104" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="104" t="s">
+      <c r="C24" s="101" t="s">
         <v>1045</v>
       </c>
-      <c r="D24" s="105" t="s">
+      <c r="D24" s="102" t="s">
         <v>1046</v>
       </c>
       <c r="E24" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="106" t="s">
+      <c r="F24" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="106" t="s">
+      <c r="G24" s="103" t="s">
         <v>56</v>
       </c>
       <c r="H24" s="21" t="s">
@@ -18376,7 +18364,7 @@
       <c r="I24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="105" t="s">
+      <c r="J24" s="102" t="s">
         <v>1046</v>
       </c>
       <c r="K24" s="19" t="s">
@@ -18388,22 +18376,22 @@
         <f aca="false">A24+1</f>
         <v>18</v>
       </c>
-      <c r="B25" s="107" t="s">
+      <c r="B25" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="104" t="s">
+      <c r="C25" s="101" t="s">
         <v>1047</v>
       </c>
-      <c r="D25" s="105" t="s">
+      <c r="D25" s="102" t="s">
         <v>1048</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="106" t="s">
+      <c r="F25" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="106" t="s">
+      <c r="G25" s="103" t="s">
         <v>1049</v>
       </c>
       <c r="H25" s="21" t="s">
@@ -18412,7 +18400,7 @@
       <c r="I25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="105" t="s">
+      <c r="J25" s="102" t="s">
         <v>1048</v>
       </c>
       <c r="K25" s="19" t="s">
@@ -18424,13 +18412,13 @@
         <f aca="false">A25+1</f>
         <v>19</v>
       </c>
-      <c r="B26" s="108" t="s">
+      <c r="B26" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="109" t="s">
+      <c r="C26" s="106" t="s">
         <v>1050</v>
       </c>
-      <c r="D26" s="110" t="s">
+      <c r="D26" s="107" t="s">
         <v>1051</v>
       </c>
       <c r="E26" s="29" t="s">
@@ -18439,7 +18427,7 @@
       <c r="F26" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="111" t="s">
+      <c r="G26" s="108" t="s">
         <v>17</v>
       </c>
       <c r="H26" s="32" t="s">
@@ -18448,7 +18436,7 @@
       <c r="I26" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="110" t="s">
+      <c r="J26" s="107" t="s">
         <v>1051</v>
       </c>
       <c r="K26" s="30" t="s">
@@ -18460,31 +18448,31 @@
         <f aca="false">A26+1</f>
         <v>20</v>
       </c>
-      <c r="B27" s="112" t="s">
+      <c r="B27" s="109" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="112" t="s">
+      <c r="C27" s="109" t="s">
         <v>1052</v>
       </c>
-      <c r="D27" s="113" t="s">
+      <c r="D27" s="110" t="s">
         <v>1053</v>
       </c>
-      <c r="E27" s="114" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="111" t="s">
+      <c r="E27" s="111" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="108" t="s">
         <v>143</v>
       </c>
-      <c r="G27" s="114" t="s">
+      <c r="G27" s="111" t="s">
         <v>1054</v>
       </c>
-      <c r="H27" s="114" t="s">
+      <c r="H27" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="114" t="s">
+      <c r="I27" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="113" t="s">
+      <c r="J27" s="110" t="s">
         <v>1055</v>
       </c>
       <c r="K27" s="30" t="s">
@@ -18496,31 +18484,31 @@
         <f aca="false">A27+1</f>
         <v>21</v>
       </c>
-      <c r="B28" s="112" t="s">
+      <c r="B28" s="109" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="112" t="s">
+      <c r="C28" s="109" t="s">
         <v>1056</v>
       </c>
-      <c r="D28" s="113" t="s">
+      <c r="D28" s="110" t="s">
         <v>1057</v>
       </c>
-      <c r="E28" s="114" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="111" t="s">
+      <c r="E28" s="111" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="108" t="s">
         <v>143</v>
       </c>
-      <c r="G28" s="114" t="s">
+      <c r="G28" s="111" t="s">
         <v>1054</v>
       </c>
-      <c r="H28" s="114" t="s">
+      <c r="H28" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="114" t="s">
+      <c r="I28" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="113" t="s">
+      <c r="J28" s="110" t="s">
         <v>1058</v>
       </c>
       <c r="K28" s="30" t="s">
@@ -18537,7 +18525,7 @@
     <mergeCell ref="A7:K7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
Ajuste no campo chaveAcesso
Ajustada a obrigatoriedade do campo chaveAcesso , que conforme a SEFAZ é obrigatório.
</commit_message>
<xml_diff>
--- a/Emissão/Layouts/LAYOUT 3.0 MDFe.xlsx
+++ b/Emissão/Layouts/LAYOUT 3.0 MDFe.xlsx
@@ -21,6 +21,30 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="J245" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">A cahve de acesso do documento (NF-e ou CT-e) é obrigatorio</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3470,7 +3494,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3819,6 +3843,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3999,8 +4027,8 @@
   </sheetPr>
   <dimension ref="A1:S363"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A262" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D267" activeCellId="0" sqref="D267"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J234" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J244" activeCellId="0" sqref="J244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13446,38 +13474,38 @@
       <c r="S244" s="7"/>
     </row>
     <row r="245" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="39" t="n">
+      <c r="A245" s="87" t="n">
         <f aca="false">A244+1</f>
         <v>203</v>
       </c>
-      <c r="B245" s="40" t="s">
+      <c r="B245" s="68" t="s">
         <v>708</v>
       </c>
-      <c r="C245" s="41" t="s">
+      <c r="C245" s="69" t="s">
         <v>709</v>
       </c>
-      <c r="D245" s="41" t="s">
+      <c r="D245" s="69" t="s">
         <v>710</v>
       </c>
-      <c r="E245" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F245" s="39" t="s">
+      <c r="E245" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="F245" s="87" t="s">
         <v>701</v>
       </c>
-      <c r="G245" s="39" t="s">
+      <c r="G245" s="87" t="s">
         <v>711</v>
       </c>
-      <c r="H245" s="42" t="s">
+      <c r="H245" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="I245" s="39" t="s">
+      <c r="I245" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="J245" s="41" t="s">
+      <c r="J245" s="69" t="s">
         <v>712</v>
       </c>
-      <c r="K245" s="40" t="s">
+      <c r="K245" s="68" t="s">
         <v>20</v>
       </c>
       <c r="L245" s="7"/>
@@ -14681,19 +14709,19 @@
       <c r="S275" s="7"/>
     </row>
     <row r="276" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="87" t="s">
+      <c r="A276" s="88" t="s">
         <v>810</v>
       </c>
-      <c r="B276" s="87"/>
-      <c r="C276" s="87"/>
-      <c r="D276" s="87"/>
-      <c r="E276" s="87"/>
-      <c r="F276" s="87"/>
-      <c r="G276" s="87"/>
-      <c r="H276" s="87"/>
-      <c r="I276" s="87"/>
-      <c r="J276" s="87"/>
-      <c r="K276" s="87"/>
+      <c r="B276" s="88"/>
+      <c r="C276" s="88"/>
+      <c r="D276" s="88"/>
+      <c r="E276" s="88"/>
+      <c r="F276" s="88"/>
+      <c r="G276" s="88"/>
+      <c r="H276" s="88"/>
+      <c r="I276" s="88"/>
+      <c r="J276" s="88"/>
+      <c r="K276" s="88"/>
     </row>
     <row r="277" s="7" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="44" t="n">
@@ -15000,7 +15028,7 @@
       <c r="I285" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J285" s="88" t="s">
+      <c r="J285" s="89" t="s">
         <v>164</v>
       </c>
       <c r="K285" s="45" t="s">
@@ -15036,7 +15064,7 @@
       <c r="I286" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J286" s="88"/>
+      <c r="J286" s="89"/>
       <c r="K286" s="45" t="s">
         <v>76</v>
       </c>
@@ -15147,16 +15175,16 @@
     </row>
     <row r="290" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="9"/>
-      <c r="B290" s="89"/>
-      <c r="C290" s="90"/>
-      <c r="D290" s="90"/>
+      <c r="B290" s="90"/>
+      <c r="C290" s="91"/>
+      <c r="D290" s="91"/>
       <c r="E290" s="9"/>
       <c r="F290" s="9"/>
       <c r="G290" s="9"/>
-      <c r="H290" s="91"/>
+      <c r="H290" s="92"/>
       <c r="I290" s="9"/>
-      <c r="J290" s="89"/>
-      <c r="K290" s="89"/>
+      <c r="J290" s="90"/>
+      <c r="K290" s="90"/>
     </row>
     <row r="291" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="12" t="s">
@@ -15202,19 +15230,19 @@
       <c r="S291" s="7"/>
     </row>
     <row r="292" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="87" t="s">
+      <c r="A292" s="88" t="s">
         <v>852</v>
       </c>
-      <c r="B292" s="87"/>
-      <c r="C292" s="87"/>
-      <c r="D292" s="87"/>
-      <c r="E292" s="87"/>
-      <c r="F292" s="87"/>
-      <c r="G292" s="87"/>
-      <c r="H292" s="87"/>
-      <c r="I292" s="87"/>
-      <c r="J292" s="87"/>
-      <c r="K292" s="87"/>
+      <c r="B292" s="88"/>
+      <c r="C292" s="88"/>
+      <c r="D292" s="88"/>
+      <c r="E292" s="88"/>
+      <c r="F292" s="88"/>
+      <c r="G292" s="88"/>
+      <c r="H292" s="88"/>
+      <c r="I292" s="88"/>
+      <c r="J292" s="88"/>
+      <c r="K292" s="88"/>
     </row>
     <row r="293" s="7" customFormat="true" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="44" t="n">
@@ -15527,7 +15555,7 @@
       <c r="I301" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J301" s="92" t="s">
+      <c r="J301" s="93" t="s">
         <v>886</v>
       </c>
       <c r="K301" s="45" t="s">
@@ -15563,7 +15591,7 @@
       <c r="I302" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J302" s="92"/>
+      <c r="J302" s="93"/>
       <c r="K302" s="45" t="s">
         <v>76</v>
       </c>
@@ -15667,7 +15695,7 @@
       <c r="I305" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J305" s="92" t="s">
+      <c r="J305" s="93" t="s">
         <v>886</v>
       </c>
       <c r="K305" s="45" t="s">
@@ -15703,23 +15731,23 @@
       <c r="I306" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J306" s="92"/>
+      <c r="J306" s="93"/>
       <c r="K306" s="45" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="307" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="9"/>
-      <c r="B307" s="89"/>
-      <c r="C307" s="90"/>
-      <c r="D307" s="90"/>
+      <c r="B307" s="90"/>
+      <c r="C307" s="91"/>
+      <c r="D307" s="91"/>
       <c r="E307" s="9"/>
       <c r="F307" s="9"/>
       <c r="G307" s="9"/>
-      <c r="H307" s="91"/>
+      <c r="H307" s="92"/>
       <c r="I307" s="9"/>
-      <c r="J307" s="89"/>
-      <c r="K307" s="89"/>
+      <c r="J307" s="90"/>
+      <c r="K307" s="90"/>
     </row>
     <row r="308" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="12" t="s">
@@ -16797,19 +16825,19 @@
       <c r="S336" s="7"/>
     </row>
     <row r="337" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="87" t="s">
+      <c r="A337" s="88" t="s">
         <v>969</v>
       </c>
-      <c r="B337" s="87"/>
-      <c r="C337" s="87"/>
-      <c r="D337" s="87"/>
-      <c r="E337" s="87"/>
-      <c r="F337" s="87"/>
-      <c r="G337" s="87"/>
-      <c r="H337" s="87"/>
-      <c r="I337" s="87"/>
-      <c r="J337" s="87"/>
-      <c r="K337" s="87"/>
+      <c r="B337" s="88"/>
+      <c r="C337" s="88"/>
+      <c r="D337" s="88"/>
+      <c r="E337" s="88"/>
+      <c r="F337" s="88"/>
+      <c r="G337" s="88"/>
+      <c r="H337" s="88"/>
+      <c r="I337" s="88"/>
+      <c r="J337" s="88"/>
+      <c r="K337" s="88"/>
       <c r="L337" s="7"/>
       <c r="M337" s="7"/>
       <c r="N337" s="7"/>
@@ -16947,19 +16975,19 @@
       <c r="S340" s="7"/>
     </row>
     <row r="341" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="87" t="s">
+      <c r="A341" s="88" t="s">
         <v>977</v>
       </c>
-      <c r="B341" s="87"/>
-      <c r="C341" s="87"/>
-      <c r="D341" s="87"/>
-      <c r="E341" s="87"/>
-      <c r="F341" s="87"/>
-      <c r="G341" s="87"/>
-      <c r="H341" s="87"/>
-      <c r="I341" s="87"/>
-      <c r="J341" s="87"/>
-      <c r="K341" s="87"/>
+      <c r="B341" s="88"/>
+      <c r="C341" s="88"/>
+      <c r="D341" s="88"/>
+      <c r="E341" s="88"/>
+      <c r="F341" s="88"/>
+      <c r="G341" s="88"/>
+      <c r="H341" s="88"/>
+      <c r="I341" s="88"/>
+      <c r="J341" s="88"/>
+      <c r="K341" s="88"/>
       <c r="L341" s="7"/>
       <c r="M341" s="7"/>
       <c r="N341" s="7"/>
@@ -17268,15 +17296,15 @@
       <c r="S348" s="7"/>
     </row>
     <row r="349" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="93"/>
+      <c r="A349" s="94"/>
       <c r="B349" s="7"/>
-      <c r="C349" s="94"/>
-      <c r="D349" s="94"/>
-      <c r="E349" s="93"/>
-      <c r="F349" s="93"/>
-      <c r="G349" s="93"/>
-      <c r="H349" s="95"/>
-      <c r="I349" s="93"/>
+      <c r="C349" s="95"/>
+      <c r="D349" s="95"/>
+      <c r="E349" s="94"/>
+      <c r="F349" s="94"/>
+      <c r="G349" s="94"/>
+      <c r="H349" s="96"/>
+      <c r="I349" s="94"/>
       <c r="J349" s="7"/>
       <c r="K349" s="7"/>
       <c r="L349" s="7"/>
@@ -17289,15 +17317,15 @@
       <c r="S349" s="7"/>
     </row>
     <row r="350" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="93"/>
+      <c r="A350" s="94"/>
       <c r="B350" s="7"/>
-      <c r="C350" s="94"/>
-      <c r="D350" s="94"/>
-      <c r="E350" s="93"/>
-      <c r="F350" s="93"/>
-      <c r="G350" s="93"/>
-      <c r="H350" s="95"/>
-      <c r="I350" s="93"/>
+      <c r="C350" s="95"/>
+      <c r="D350" s="95"/>
+      <c r="E350" s="94"/>
+      <c r="F350" s="94"/>
+      <c r="G350" s="94"/>
+      <c r="H350" s="96"/>
+      <c r="I350" s="94"/>
       <c r="J350" s="7"/>
       <c r="K350" s="7"/>
       <c r="L350" s="7"/>
@@ -17310,15 +17338,15 @@
       <c r="S350" s="7"/>
     </row>
     <row r="351" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="93"/>
+      <c r="A351" s="94"/>
       <c r="B351" s="7"/>
-      <c r="C351" s="94"/>
-      <c r="D351" s="94"/>
-      <c r="E351" s="93"/>
-      <c r="F351" s="93"/>
-      <c r="G351" s="93"/>
-      <c r="H351" s="95"/>
-      <c r="I351" s="93"/>
+      <c r="C351" s="95"/>
+      <c r="D351" s="95"/>
+      <c r="E351" s="94"/>
+      <c r="F351" s="94"/>
+      <c r="G351" s="94"/>
+      <c r="H351" s="96"/>
+      <c r="I351" s="94"/>
       <c r="J351" s="7"/>
       <c r="K351" s="7"/>
       <c r="L351" s="7"/>
@@ -17331,15 +17359,15 @@
       <c r="S351" s="7"/>
     </row>
     <row r="352" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="93"/>
+      <c r="A352" s="94"/>
       <c r="B352" s="7"/>
-      <c r="C352" s="94"/>
-      <c r="D352" s="94"/>
-      <c r="E352" s="93"/>
-      <c r="F352" s="93"/>
-      <c r="G352" s="93"/>
-      <c r="H352" s="95"/>
-      <c r="I352" s="93"/>
+      <c r="C352" s="95"/>
+      <c r="D352" s="95"/>
+      <c r="E352" s="94"/>
+      <c r="F352" s="94"/>
+      <c r="G352" s="94"/>
+      <c r="H352" s="96"/>
+      <c r="I352" s="94"/>
       <c r="J352" s="7"/>
       <c r="K352" s="7"/>
       <c r="L352" s="7"/>
@@ -17352,15 +17380,15 @@
       <c r="S352" s="7"/>
     </row>
     <row r="353" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="93"/>
+      <c r="A353" s="94"/>
       <c r="B353" s="7"/>
-      <c r="C353" s="94"/>
-      <c r="D353" s="94"/>
-      <c r="E353" s="93"/>
-      <c r="F353" s="93"/>
-      <c r="G353" s="93"/>
-      <c r="H353" s="95"/>
-      <c r="I353" s="93"/>
+      <c r="C353" s="95"/>
+      <c r="D353" s="95"/>
+      <c r="E353" s="94"/>
+      <c r="F353" s="94"/>
+      <c r="G353" s="94"/>
+      <c r="H353" s="96"/>
+      <c r="I353" s="94"/>
       <c r="J353" s="7"/>
       <c r="K353" s="7"/>
       <c r="L353" s="7"/>
@@ -17373,15 +17401,15 @@
       <c r="S353" s="7"/>
     </row>
     <row r="354" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="93"/>
+      <c r="A354" s="94"/>
       <c r="B354" s="7"/>
-      <c r="C354" s="94"/>
-      <c r="D354" s="94"/>
-      <c r="E354" s="93"/>
-      <c r="F354" s="93"/>
-      <c r="G354" s="93"/>
-      <c r="H354" s="95"/>
-      <c r="I354" s="93"/>
+      <c r="C354" s="95"/>
+      <c r="D354" s="95"/>
+      <c r="E354" s="94"/>
+      <c r="F354" s="94"/>
+      <c r="G354" s="94"/>
+      <c r="H354" s="96"/>
+      <c r="I354" s="94"/>
       <c r="J354" s="7"/>
       <c r="K354" s="7"/>
       <c r="L354" s="7"/>
@@ -17394,15 +17422,15 @@
       <c r="S354" s="7"/>
     </row>
     <row r="355" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="93"/>
+      <c r="A355" s="94"/>
       <c r="B355" s="7"/>
-      <c r="C355" s="94"/>
-      <c r="D355" s="94"/>
-      <c r="E355" s="93"/>
-      <c r="F355" s="93"/>
-      <c r="G355" s="93"/>
-      <c r="H355" s="95"/>
-      <c r="I355" s="93"/>
+      <c r="C355" s="95"/>
+      <c r="D355" s="95"/>
+      <c r="E355" s="94"/>
+      <c r="F355" s="94"/>
+      <c r="G355" s="94"/>
+      <c r="H355" s="96"/>
+      <c r="I355" s="94"/>
       <c r="J355" s="7"/>
       <c r="K355" s="7"/>
       <c r="L355" s="7"/>
@@ -17415,15 +17443,15 @@
       <c r="S355" s="7"/>
     </row>
     <row r="356" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="93"/>
+      <c r="A356" s="94"/>
       <c r="B356" s="7"/>
-      <c r="C356" s="94"/>
-      <c r="D356" s="94"/>
-      <c r="E356" s="93"/>
-      <c r="F356" s="93"/>
-      <c r="G356" s="93"/>
-      <c r="H356" s="95"/>
-      <c r="I356" s="93"/>
+      <c r="C356" s="95"/>
+      <c r="D356" s="95"/>
+      <c r="E356" s="94"/>
+      <c r="F356" s="94"/>
+      <c r="G356" s="94"/>
+      <c r="H356" s="96"/>
+      <c r="I356" s="94"/>
       <c r="J356" s="7"/>
       <c r="K356" s="7"/>
       <c r="L356" s="7"/>
@@ -17436,15 +17464,15 @@
       <c r="S356" s="7"/>
     </row>
     <row r="357" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="93"/>
+      <c r="A357" s="94"/>
       <c r="B357" s="7"/>
-      <c r="C357" s="94"/>
-      <c r="D357" s="94"/>
-      <c r="E357" s="93"/>
-      <c r="F357" s="93"/>
-      <c r="G357" s="93"/>
-      <c r="H357" s="95"/>
-      <c r="I357" s="93"/>
+      <c r="C357" s="95"/>
+      <c r="D357" s="95"/>
+      <c r="E357" s="94"/>
+      <c r="F357" s="94"/>
+      <c r="G357" s="94"/>
+      <c r="H357" s="96"/>
+      <c r="I357" s="94"/>
       <c r="J357" s="7"/>
       <c r="K357" s="7"/>
       <c r="L357" s="7"/>
@@ -17457,15 +17485,15 @@
       <c r="S357" s="7"/>
     </row>
     <row r="358" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="93"/>
+      <c r="A358" s="94"/>
       <c r="B358" s="7"/>
-      <c r="C358" s="94"/>
-      <c r="D358" s="94"/>
-      <c r="E358" s="93"/>
-      <c r="F358" s="93"/>
-      <c r="G358" s="93"/>
-      <c r="H358" s="95"/>
-      <c r="I358" s="93"/>
+      <c r="C358" s="95"/>
+      <c r="D358" s="95"/>
+      <c r="E358" s="94"/>
+      <c r="F358" s="94"/>
+      <c r="G358" s="94"/>
+      <c r="H358" s="96"/>
+      <c r="I358" s="94"/>
       <c r="J358" s="7"/>
       <c r="K358" s="7"/>
       <c r="L358" s="7"/>
@@ -17478,15 +17506,15 @@
       <c r="S358" s="7"/>
     </row>
     <row r="359" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="93"/>
+      <c r="A359" s="94"/>
       <c r="B359" s="7"/>
-      <c r="C359" s="94"/>
-      <c r="D359" s="94"/>
-      <c r="E359" s="93"/>
-      <c r="F359" s="93"/>
-      <c r="G359" s="93"/>
-      <c r="H359" s="95"/>
-      <c r="I359" s="93"/>
+      <c r="C359" s="95"/>
+      <c r="D359" s="95"/>
+      <c r="E359" s="94"/>
+      <c r="F359" s="94"/>
+      <c r="G359" s="94"/>
+      <c r="H359" s="96"/>
+      <c r="I359" s="94"/>
       <c r="J359" s="7"/>
       <c r="K359" s="7"/>
       <c r="L359" s="7"/>
@@ -17499,15 +17527,15 @@
       <c r="S359" s="7"/>
     </row>
     <row r="360" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="93"/>
+      <c r="A360" s="94"/>
       <c r="B360" s="7"/>
-      <c r="C360" s="94"/>
-      <c r="D360" s="94"/>
-      <c r="E360" s="93"/>
-      <c r="F360" s="93"/>
-      <c r="G360" s="93"/>
-      <c r="H360" s="95"/>
-      <c r="I360" s="93"/>
+      <c r="C360" s="95"/>
+      <c r="D360" s="95"/>
+      <c r="E360" s="94"/>
+      <c r="F360" s="94"/>
+      <c r="G360" s="94"/>
+      <c r="H360" s="96"/>
+      <c r="I360" s="94"/>
       <c r="J360" s="7"/>
       <c r="K360" s="7"/>
       <c r="L360" s="7"/>
@@ -17520,15 +17548,15 @@
       <c r="S360" s="7"/>
     </row>
     <row r="361" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="93"/>
+      <c r="A361" s="94"/>
       <c r="B361" s="7"/>
-      <c r="C361" s="94"/>
-      <c r="D361" s="94"/>
-      <c r="E361" s="93"/>
-      <c r="F361" s="93"/>
-      <c r="G361" s="93"/>
-      <c r="H361" s="95"/>
-      <c r="I361" s="93"/>
+      <c r="C361" s="95"/>
+      <c r="D361" s="95"/>
+      <c r="E361" s="94"/>
+      <c r="F361" s="94"/>
+      <c r="G361" s="94"/>
+      <c r="H361" s="96"/>
+      <c r="I361" s="94"/>
       <c r="J361" s="7"/>
       <c r="K361" s="7"/>
       <c r="L361" s="7"/>
@@ -17541,15 +17569,15 @@
       <c r="S361" s="7"/>
     </row>
     <row r="362" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="93"/>
+      <c r="A362" s="94"/>
       <c r="B362" s="7"/>
-      <c r="C362" s="94"/>
-      <c r="D362" s="94"/>
-      <c r="E362" s="93"/>
-      <c r="F362" s="93"/>
-      <c r="G362" s="93"/>
-      <c r="H362" s="95"/>
-      <c r="I362" s="93"/>
+      <c r="C362" s="95"/>
+      <c r="D362" s="95"/>
+      <c r="E362" s="94"/>
+      <c r="F362" s="94"/>
+      <c r="G362" s="94"/>
+      <c r="H362" s="96"/>
+      <c r="I362" s="94"/>
       <c r="J362" s="7"/>
       <c r="K362" s="7"/>
       <c r="L362" s="7"/>
@@ -17608,10 +17636,10 @@
     <mergeCell ref="A341:K341"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J21" r:id="rId1" display="Consulte nosso artigo para mais informações."/>
-    <hyperlink ref="J41" r:id="rId2" display="Consulte nosso artigo para mais informações."/>
-    <hyperlink ref="J63" r:id="rId3" display="Consulte nosso artigo para mais informações."/>
-    <hyperlink ref="J240" r:id="rId4" display="Consulte nosso artigo para mais informações."/>
+    <hyperlink ref="J21" r:id="rId2" display="Consulte nosso artigo para mais informações."/>
+    <hyperlink ref="J41" r:id="rId3" display="Consulte nosso artigo para mais informações."/>
+    <hyperlink ref="J63" r:id="rId4" display="Consulte nosso artigo para mais informações."/>
+    <hyperlink ref="J240" r:id="rId5" display="Consulte nosso artigo para mais informações."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
@@ -17620,6 +17648,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -17636,11 +17665,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="96" width="6.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="96" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="96" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="96" width="36.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="96" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="97" width="6.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="97" width="17.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="97" width="40.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="97" width="36.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="97" width="7.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17687,28 +17716,28 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
@@ -17746,19 +17775,19 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="99" t="s">
         <v>1003</v>
       </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="n">
@@ -17767,7 +17796,7 @@
       <c r="B8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="99" t="s">
+      <c r="C8" s="100" t="s">
         <v>1004</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -17803,7 +17832,7 @@
       <c r="B9" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="101" t="s">
         <v>1006</v>
       </c>
       <c r="D9" s="25" t="s">
@@ -17839,7 +17868,7 @@
       <c r="B10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="100" t="s">
         <v>1008</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -17875,10 +17904,10 @@
       <c r="B11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="101" t="s">
+      <c r="C11" s="102" t="s">
         <v>1010</v>
       </c>
-      <c r="D11" s="102" t="s">
+      <c r="D11" s="103" t="s">
         <v>1011</v>
       </c>
       <c r="E11" s="24" t="s">
@@ -17887,7 +17916,7 @@
       <c r="F11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="103" t="s">
+      <c r="G11" s="104" t="s">
         <v>997</v>
       </c>
       <c r="H11" s="21" t="s">
@@ -17896,7 +17925,7 @@
       <c r="I11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="102" t="s">
+      <c r="J11" s="103" t="s">
         <v>1011</v>
       </c>
       <c r="K11" s="19" t="s">
@@ -17911,10 +17940,10 @@
       <c r="B12" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="101" t="s">
+      <c r="C12" s="102" t="s">
         <v>1012</v>
       </c>
-      <c r="D12" s="102" t="s">
+      <c r="D12" s="103" t="s">
         <v>1013</v>
       </c>
       <c r="E12" s="24" t="s">
@@ -17923,7 +17952,7 @@
       <c r="F12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="103" t="s">
+      <c r="G12" s="104" t="s">
         <v>711</v>
       </c>
       <c r="H12" s="21" t="s">
@@ -17932,7 +17961,7 @@
       <c r="I12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="102" t="s">
+      <c r="J12" s="103" t="s">
         <v>1013</v>
       </c>
       <c r="K12" s="19" t="s">
@@ -17947,10 +17976,10 @@
       <c r="B13" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="101" t="s">
+      <c r="C13" s="102" t="s">
         <v>1014</v>
       </c>
-      <c r="D13" s="102" t="s">
+      <c r="D13" s="103" t="s">
         <v>1015</v>
       </c>
       <c r="E13" s="24" t="s">
@@ -17959,7 +17988,7 @@
       <c r="F13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="103" t="s">
+      <c r="G13" s="104" t="s">
         <v>267</v>
       </c>
       <c r="H13" s="21" t="s">
@@ -17968,7 +17997,7 @@
       <c r="I13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="102" t="s">
+      <c r="J13" s="103" t="s">
         <v>1015</v>
       </c>
       <c r="K13" s="19" t="s">
@@ -17983,10 +18012,10 @@
       <c r="B14" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="101" t="s">
+      <c r="C14" s="102" t="s">
         <v>1016</v>
       </c>
-      <c r="D14" s="102" t="s">
+      <c r="D14" s="103" t="s">
         <v>1017</v>
       </c>
       <c r="E14" s="24" t="s">
@@ -17995,7 +18024,7 @@
       <c r="F14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="103" t="s">
+      <c r="G14" s="104" t="s">
         <v>61</v>
       </c>
       <c r="H14" s="21" t="s">
@@ -18004,7 +18033,7 @@
       <c r="I14" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="102" t="s">
+      <c r="J14" s="103" t="s">
         <v>1017</v>
       </c>
       <c r="K14" s="19" t="s">
@@ -18019,10 +18048,10 @@
       <c r="B15" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="101" t="s">
+      <c r="C15" s="102" t="s">
         <v>1018</v>
       </c>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="103" t="s">
         <v>1019</v>
       </c>
       <c r="E15" s="24" t="s">
@@ -18031,7 +18060,7 @@
       <c r="F15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="103" t="s">
+      <c r="G15" s="104" t="s">
         <v>375</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -18040,7 +18069,7 @@
       <c r="I15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="102" t="s">
+      <c r="J15" s="103" t="s">
         <v>1020</v>
       </c>
       <c r="K15" s="19" t="s">
@@ -18055,10 +18084,10 @@
       <c r="B16" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="101" t="s">
+      <c r="C16" s="102" t="s">
         <v>1021</v>
       </c>
-      <c r="D16" s="102" t="s">
+      <c r="D16" s="103" t="s">
         <v>1022</v>
       </c>
       <c r="E16" s="24" t="s">
@@ -18067,7 +18096,7 @@
       <c r="F16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="103" t="s">
+      <c r="G16" s="104" t="s">
         <v>1023</v>
       </c>
       <c r="H16" s="21" t="s">
@@ -18076,7 +18105,7 @@
       <c r="I16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="102" t="s">
+      <c r="J16" s="103" t="s">
         <v>1024</v>
       </c>
       <c r="K16" s="19" t="s">
@@ -18091,10 +18120,10 @@
       <c r="B17" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="102" t="s">
         <v>1025</v>
       </c>
-      <c r="D17" s="102" t="s">
+      <c r="D17" s="103" t="s">
         <v>1026</v>
       </c>
       <c r="E17" s="24" t="s">
@@ -18103,7 +18132,7 @@
       <c r="F17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="103" t="s">
+      <c r="G17" s="104" t="s">
         <v>1027</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -18112,7 +18141,7 @@
       <c r="I17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="102" t="s">
+      <c r="J17" s="103" t="s">
         <v>1028</v>
       </c>
       <c r="K17" s="19" t="s">
@@ -18127,10 +18156,10 @@
       <c r="B18" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="101" t="s">
+      <c r="C18" s="102" t="s">
         <v>1029</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="103" t="s">
         <v>1030</v>
       </c>
       <c r="E18" s="24" t="s">
@@ -18139,7 +18168,7 @@
       <c r="F18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="103" t="s">
+      <c r="G18" s="104" t="s">
         <v>1027</v>
       </c>
       <c r="H18" s="21" t="s">
@@ -18148,7 +18177,7 @@
       <c r="I18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="102" t="s">
+      <c r="J18" s="103" t="s">
         <v>1031</v>
       </c>
       <c r="K18" s="19" t="s">
@@ -18163,10 +18192,10 @@
       <c r="B19" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="101" t="s">
+      <c r="C19" s="102" t="s">
         <v>1032</v>
       </c>
-      <c r="D19" s="102" t="s">
+      <c r="D19" s="103" t="s">
         <v>1033</v>
       </c>
       <c r="E19" s="24" t="s">
@@ -18175,7 +18204,7 @@
       <c r="F19" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="103" t="s">
+      <c r="G19" s="104" t="s">
         <v>1027</v>
       </c>
       <c r="H19" s="21" t="s">
@@ -18184,7 +18213,7 @@
       <c r="I19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="102" t="s">
+      <c r="J19" s="103" t="s">
         <v>1034</v>
       </c>
       <c r="K19" s="19" t="s">
@@ -18199,10 +18228,10 @@
       <c r="B20" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="102" t="s">
         <v>1035</v>
       </c>
-      <c r="D20" s="102" t="s">
+      <c r="D20" s="103" t="s">
         <v>1036</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -18211,7 +18240,7 @@
       <c r="F20" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="103" t="s">
+      <c r="G20" s="104" t="s">
         <v>1027</v>
       </c>
       <c r="H20" s="21" t="s">
@@ -18220,7 +18249,7 @@
       <c r="I20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="102" t="s">
+      <c r="J20" s="103" t="s">
         <v>1036</v>
       </c>
       <c r="K20" s="19" t="s">
@@ -18235,10 +18264,10 @@
       <c r="B21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="101" t="s">
+      <c r="C21" s="102" t="s">
         <v>1037</v>
       </c>
-      <c r="D21" s="102" t="s">
+      <c r="D21" s="103" t="s">
         <v>1038</v>
       </c>
       <c r="E21" s="24" t="s">
@@ -18247,7 +18276,7 @@
       <c r="F21" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="103" t="s">
+      <c r="G21" s="104" t="s">
         <v>1027</v>
       </c>
       <c r="H21" s="21" t="s">
@@ -18256,7 +18285,7 @@
       <c r="I21" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="102" t="s">
+      <c r="J21" s="103" t="s">
         <v>1038</v>
       </c>
       <c r="K21" s="19" t="s">
@@ -18271,10 +18300,10 @@
       <c r="B22" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="101" t="s">
+      <c r="C22" s="102" t="s">
         <v>1039</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="103" t="s">
         <v>1040</v>
       </c>
       <c r="E22" s="24" t="s">
@@ -18283,7 +18312,7 @@
       <c r="F22" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="103" t="s">
+      <c r="G22" s="104" t="s">
         <v>1041</v>
       </c>
       <c r="H22" s="21" t="s">
@@ -18292,7 +18321,7 @@
       <c r="I22" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="102" t="s">
+      <c r="J22" s="103" t="s">
         <v>1042</v>
       </c>
       <c r="K22" s="19" t="s">
@@ -18304,13 +18333,13 @@
         <f aca="false">A22+1</f>
         <v>16</v>
       </c>
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="105" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="102" t="s">
         <v>1043</v>
       </c>
-      <c r="D23" s="102" t="s">
+      <c r="D23" s="103" t="s">
         <v>1044</v>
       </c>
       <c r="E23" s="18" t="s">
@@ -18319,7 +18348,7 @@
       <c r="F23" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="103" t="s">
+      <c r="G23" s="104" t="s">
         <v>17</v>
       </c>
       <c r="H23" s="21" t="s">
@@ -18328,7 +18357,7 @@
       <c r="I23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="102" t="s">
+      <c r="J23" s="103" t="s">
         <v>1044</v>
       </c>
       <c r="K23" s="19" t="s">
@@ -18340,22 +18369,22 @@
         <f aca="false">A23+1</f>
         <v>17</v>
       </c>
-      <c r="B24" s="104" t="s">
+      <c r="B24" s="105" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="102" t="s">
         <v>1045</v>
       </c>
-      <c r="D24" s="102" t="s">
+      <c r="D24" s="103" t="s">
         <v>1046</v>
       </c>
       <c r="E24" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="103" t="s">
+      <c r="F24" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="103" t="s">
+      <c r="G24" s="104" t="s">
         <v>56</v>
       </c>
       <c r="H24" s="21" t="s">
@@ -18364,7 +18393,7 @@
       <c r="I24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="102" t="s">
+      <c r="J24" s="103" t="s">
         <v>1046</v>
       </c>
       <c r="K24" s="19" t="s">
@@ -18376,22 +18405,22 @@
         <f aca="false">A24+1</f>
         <v>18</v>
       </c>
-      <c r="B25" s="104" t="s">
+      <c r="B25" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="101" t="s">
+      <c r="C25" s="102" t="s">
         <v>1047</v>
       </c>
-      <c r="D25" s="102" t="s">
+      <c r="D25" s="103" t="s">
         <v>1048</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="103" t="s">
+      <c r="F25" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="103" t="s">
+      <c r="G25" s="104" t="s">
         <v>1049</v>
       </c>
       <c r="H25" s="21" t="s">
@@ -18400,7 +18429,7 @@
       <c r="I25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="102" t="s">
+      <c r="J25" s="103" t="s">
         <v>1048</v>
       </c>
       <c r="K25" s="19" t="s">
@@ -18412,13 +18441,13 @@
         <f aca="false">A25+1</f>
         <v>19</v>
       </c>
-      <c r="B26" s="105" t="s">
+      <c r="B26" s="106" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="106" t="s">
+      <c r="C26" s="107" t="s">
         <v>1050</v>
       </c>
-      <c r="D26" s="107" t="s">
+      <c r="D26" s="108" t="s">
         <v>1051</v>
       </c>
       <c r="E26" s="29" t="s">
@@ -18427,7 +18456,7 @@
       <c r="F26" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="108" t="s">
+      <c r="G26" s="109" t="s">
         <v>17</v>
       </c>
       <c r="H26" s="32" t="s">
@@ -18436,7 +18465,7 @@
       <c r="I26" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="107" t="s">
+      <c r="J26" s="108" t="s">
         <v>1051</v>
       </c>
       <c r="K26" s="30" t="s">
@@ -18448,31 +18477,31 @@
         <f aca="false">A26+1</f>
         <v>20</v>
       </c>
-      <c r="B27" s="109" t="s">
+      <c r="B27" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="109" t="s">
+      <c r="C27" s="110" t="s">
         <v>1052</v>
       </c>
-      <c r="D27" s="110" t="s">
+      <c r="D27" s="111" t="s">
         <v>1053</v>
       </c>
-      <c r="E27" s="111" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="108" t="s">
+      <c r="E27" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="G27" s="111" t="s">
+      <c r="G27" s="112" t="s">
         <v>1054</v>
       </c>
-      <c r="H27" s="111" t="s">
+      <c r="H27" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="111" t="s">
+      <c r="I27" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="110" t="s">
+      <c r="J27" s="111" t="s">
         <v>1055</v>
       </c>
       <c r="K27" s="30" t="s">
@@ -18484,31 +18513,31 @@
         <f aca="false">A27+1</f>
         <v>21</v>
       </c>
-      <c r="B28" s="109" t="s">
+      <c r="B28" s="110" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="109" t="s">
+      <c r="C28" s="110" t="s">
         <v>1056</v>
       </c>
-      <c r="D28" s="110" t="s">
+      <c r="D28" s="111" t="s">
         <v>1057</v>
       </c>
-      <c r="E28" s="111" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="108" t="s">
+      <c r="E28" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="109" t="s">
         <v>143</v>
       </c>
-      <c r="G28" s="111" t="s">
+      <c r="G28" s="112" t="s">
         <v>1054</v>
       </c>
-      <c r="H28" s="111" t="s">
+      <c r="H28" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="111" t="s">
+      <c r="I28" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="110" t="s">
+      <c r="J28" s="111" t="s">
         <v>1058</v>
       </c>
       <c r="K28" s="30" t="s">

</xml_diff>

<commit_message>
Ajuste nas Tags DocPDFDownload e DocXMLDownload
Tamanho padronizado em 999
</commit_message>
<xml_diff>
--- a/Emissão/Layouts/LAYOUT 3.0 MDFe.xlsx
+++ b/Emissão/Layouts/LAYOUT 3.0 MDFe.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="1061">
   <si>
     <t xml:space="preserve">LAYOUT 3.0 - MDF-e</t>
   </si>
@@ -3232,10 +3232,16 @@
     <t xml:space="preserve">Link para download do PDF do documento</t>
   </si>
   <si>
+    <t xml:space="preserve">V(999))</t>
+  </si>
+  <si>
     <t xml:space="preserve"> DocXMLDownload</t>
   </si>
   <si>
     <t xml:space="preserve">Link para download do arquivo XML do documento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V(999)</t>
   </si>
   <si>
     <t xml:space="preserve">DocImpressora</t>
@@ -3308,7 +3314,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="d/mmm"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3381,6 +3387,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3843,10 +3854,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3912,6 +3919,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4027,7 +4038,7 @@
   </sheetPr>
   <dimension ref="A1:S363"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J234" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J244" activeCellId="0" sqref="J244"/>
     </sheetView>
   </sheetViews>
@@ -13474,7 +13485,7 @@
       <c r="S244" s="7"/>
     </row>
     <row r="245" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="87" t="n">
+      <c r="A245" s="67" t="n">
         <f aca="false">A244+1</f>
         <v>203</v>
       </c>
@@ -13487,19 +13498,19 @@
       <c r="D245" s="69" t="s">
         <v>710</v>
       </c>
-      <c r="E245" s="87" t="s">
-        <v>23</v>
-      </c>
-      <c r="F245" s="87" t="s">
+      <c r="E245" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="F245" s="67" t="s">
         <v>701</v>
       </c>
-      <c r="G245" s="87" t="s">
+      <c r="G245" s="67" t="s">
         <v>711</v>
       </c>
       <c r="H245" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="I245" s="87" t="s">
+      <c r="I245" s="67" t="s">
         <v>35</v>
       </c>
       <c r="J245" s="69" t="s">
@@ -14709,19 +14720,19 @@
       <c r="S275" s="7"/>
     </row>
     <row r="276" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="88" t="s">
+      <c r="A276" s="87" t="s">
         <v>810</v>
       </c>
-      <c r="B276" s="88"/>
-      <c r="C276" s="88"/>
-      <c r="D276" s="88"/>
-      <c r="E276" s="88"/>
-      <c r="F276" s="88"/>
-      <c r="G276" s="88"/>
-      <c r="H276" s="88"/>
-      <c r="I276" s="88"/>
-      <c r="J276" s="88"/>
-      <c r="K276" s="88"/>
+      <c r="B276" s="87"/>
+      <c r="C276" s="87"/>
+      <c r="D276" s="87"/>
+      <c r="E276" s="87"/>
+      <c r="F276" s="87"/>
+      <c r="G276" s="87"/>
+      <c r="H276" s="87"/>
+      <c r="I276" s="87"/>
+      <c r="J276" s="87"/>
+      <c r="K276" s="87"/>
     </row>
     <row r="277" s="7" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="44" t="n">
@@ -15028,7 +15039,7 @@
       <c r="I285" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J285" s="89" t="s">
+      <c r="J285" s="88" t="s">
         <v>164</v>
       </c>
       <c r="K285" s="45" t="s">
@@ -15064,7 +15075,7 @@
       <c r="I286" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J286" s="89"/>
+      <c r="J286" s="88"/>
       <c r="K286" s="45" t="s">
         <v>76</v>
       </c>
@@ -15175,16 +15186,16 @@
     </row>
     <row r="290" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="9"/>
-      <c r="B290" s="90"/>
-      <c r="C290" s="91"/>
-      <c r="D290" s="91"/>
+      <c r="B290" s="89"/>
+      <c r="C290" s="90"/>
+      <c r="D290" s="90"/>
       <c r="E290" s="9"/>
       <c r="F290" s="9"/>
       <c r="G290" s="9"/>
-      <c r="H290" s="92"/>
+      <c r="H290" s="91"/>
       <c r="I290" s="9"/>
-      <c r="J290" s="90"/>
-      <c r="K290" s="90"/>
+      <c r="J290" s="89"/>
+      <c r="K290" s="89"/>
     </row>
     <row r="291" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="12" t="s">
@@ -15230,19 +15241,19 @@
       <c r="S291" s="7"/>
     </row>
     <row r="292" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="88" t="s">
+      <c r="A292" s="87" t="s">
         <v>852</v>
       </c>
-      <c r="B292" s="88"/>
-      <c r="C292" s="88"/>
-      <c r="D292" s="88"/>
-      <c r="E292" s="88"/>
-      <c r="F292" s="88"/>
-      <c r="G292" s="88"/>
-      <c r="H292" s="88"/>
-      <c r="I292" s="88"/>
-      <c r="J292" s="88"/>
-      <c r="K292" s="88"/>
+      <c r="B292" s="87"/>
+      <c r="C292" s="87"/>
+      <c r="D292" s="87"/>
+      <c r="E292" s="87"/>
+      <c r="F292" s="87"/>
+      <c r="G292" s="87"/>
+      <c r="H292" s="87"/>
+      <c r="I292" s="87"/>
+      <c r="J292" s="87"/>
+      <c r="K292" s="87"/>
     </row>
     <row r="293" s="7" customFormat="true" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="44" t="n">
@@ -15555,7 +15566,7 @@
       <c r="I301" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J301" s="93" t="s">
+      <c r="J301" s="92" t="s">
         <v>886</v>
       </c>
       <c r="K301" s="45" t="s">
@@ -15591,7 +15602,7 @@
       <c r="I302" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J302" s="93"/>
+      <c r="J302" s="92"/>
       <c r="K302" s="45" t="s">
         <v>76</v>
       </c>
@@ -15695,7 +15706,7 @@
       <c r="I305" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J305" s="93" t="s">
+      <c r="J305" s="92" t="s">
         <v>886</v>
       </c>
       <c r="K305" s="45" t="s">
@@ -15731,23 +15742,23 @@
       <c r="I306" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="J306" s="93"/>
+      <c r="J306" s="92"/>
       <c r="K306" s="45" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="307" s="7" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="9"/>
-      <c r="B307" s="90"/>
-      <c r="C307" s="91"/>
-      <c r="D307" s="91"/>
+      <c r="B307" s="89"/>
+      <c r="C307" s="90"/>
+      <c r="D307" s="90"/>
       <c r="E307" s="9"/>
       <c r="F307" s="9"/>
       <c r="G307" s="9"/>
-      <c r="H307" s="92"/>
+      <c r="H307" s="91"/>
       <c r="I307" s="9"/>
-      <c r="J307" s="90"/>
-      <c r="K307" s="90"/>
+      <c r="J307" s="89"/>
+      <c r="K307" s="89"/>
     </row>
     <row r="308" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="12" t="s">
@@ -16825,19 +16836,19 @@
       <c r="S336" s="7"/>
     </row>
     <row r="337" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="88" t="s">
+      <c r="A337" s="87" t="s">
         <v>969</v>
       </c>
-      <c r="B337" s="88"/>
-      <c r="C337" s="88"/>
-      <c r="D337" s="88"/>
-      <c r="E337" s="88"/>
-      <c r="F337" s="88"/>
-      <c r="G337" s="88"/>
-      <c r="H337" s="88"/>
-      <c r="I337" s="88"/>
-      <c r="J337" s="88"/>
-      <c r="K337" s="88"/>
+      <c r="B337" s="87"/>
+      <c r="C337" s="87"/>
+      <c r="D337" s="87"/>
+      <c r="E337" s="87"/>
+      <c r="F337" s="87"/>
+      <c r="G337" s="87"/>
+      <c r="H337" s="87"/>
+      <c r="I337" s="87"/>
+      <c r="J337" s="87"/>
+      <c r="K337" s="87"/>
       <c r="L337" s="7"/>
       <c r="M337" s="7"/>
       <c r="N337" s="7"/>
@@ -16975,19 +16986,19 @@
       <c r="S340" s="7"/>
     </row>
     <row r="341" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="88" t="s">
+      <c r="A341" s="87" t="s">
         <v>977</v>
       </c>
-      <c r="B341" s="88"/>
-      <c r="C341" s="88"/>
-      <c r="D341" s="88"/>
-      <c r="E341" s="88"/>
-      <c r="F341" s="88"/>
-      <c r="G341" s="88"/>
-      <c r="H341" s="88"/>
-      <c r="I341" s="88"/>
-      <c r="J341" s="88"/>
-      <c r="K341" s="88"/>
+      <c r="B341" s="87"/>
+      <c r="C341" s="87"/>
+      <c r="D341" s="87"/>
+      <c r="E341" s="87"/>
+      <c r="F341" s="87"/>
+      <c r="G341" s="87"/>
+      <c r="H341" s="87"/>
+      <c r="I341" s="87"/>
+      <c r="J341" s="87"/>
+      <c r="K341" s="87"/>
       <c r="L341" s="7"/>
       <c r="M341" s="7"/>
       <c r="N341" s="7"/>
@@ -17296,15 +17307,15 @@
       <c r="S348" s="7"/>
     </row>
     <row r="349" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="94"/>
+      <c r="A349" s="93"/>
       <c r="B349" s="7"/>
-      <c r="C349" s="95"/>
-      <c r="D349" s="95"/>
-      <c r="E349" s="94"/>
-      <c r="F349" s="94"/>
-      <c r="G349" s="94"/>
-      <c r="H349" s="96"/>
-      <c r="I349" s="94"/>
+      <c r="C349" s="94"/>
+      <c r="D349" s="94"/>
+      <c r="E349" s="93"/>
+      <c r="F349" s="93"/>
+      <c r="G349" s="93"/>
+      <c r="H349" s="95"/>
+      <c r="I349" s="93"/>
       <c r="J349" s="7"/>
       <c r="K349" s="7"/>
       <c r="L349" s="7"/>
@@ -17317,15 +17328,15 @@
       <c r="S349" s="7"/>
     </row>
     <row r="350" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="94"/>
+      <c r="A350" s="93"/>
       <c r="B350" s="7"/>
-      <c r="C350" s="95"/>
-      <c r="D350" s="95"/>
-      <c r="E350" s="94"/>
-      <c r="F350" s="94"/>
-      <c r="G350" s="94"/>
-      <c r="H350" s="96"/>
-      <c r="I350" s="94"/>
+      <c r="C350" s="94"/>
+      <c r="D350" s="94"/>
+      <c r="E350" s="93"/>
+      <c r="F350" s="93"/>
+      <c r="G350" s="93"/>
+      <c r="H350" s="95"/>
+      <c r="I350" s="93"/>
       <c r="J350" s="7"/>
       <c r="K350" s="7"/>
       <c r="L350" s="7"/>
@@ -17338,15 +17349,15 @@
       <c r="S350" s="7"/>
     </row>
     <row r="351" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="94"/>
+      <c r="A351" s="93"/>
       <c r="B351" s="7"/>
-      <c r="C351" s="95"/>
-      <c r="D351" s="95"/>
-      <c r="E351" s="94"/>
-      <c r="F351" s="94"/>
-      <c r="G351" s="94"/>
-      <c r="H351" s="96"/>
-      <c r="I351" s="94"/>
+      <c r="C351" s="94"/>
+      <c r="D351" s="94"/>
+      <c r="E351" s="93"/>
+      <c r="F351" s="93"/>
+      <c r="G351" s="93"/>
+      <c r="H351" s="95"/>
+      <c r="I351" s="93"/>
       <c r="J351" s="7"/>
       <c r="K351" s="7"/>
       <c r="L351" s="7"/>
@@ -17359,15 +17370,15 @@
       <c r="S351" s="7"/>
     </row>
     <row r="352" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="94"/>
+      <c r="A352" s="93"/>
       <c r="B352" s="7"/>
-      <c r="C352" s="95"/>
-      <c r="D352" s="95"/>
-      <c r="E352" s="94"/>
-      <c r="F352" s="94"/>
-      <c r="G352" s="94"/>
-      <c r="H352" s="96"/>
-      <c r="I352" s="94"/>
+      <c r="C352" s="94"/>
+      <c r="D352" s="94"/>
+      <c r="E352" s="93"/>
+      <c r="F352" s="93"/>
+      <c r="G352" s="93"/>
+      <c r="H352" s="95"/>
+      <c r="I352" s="93"/>
       <c r="J352" s="7"/>
       <c r="K352" s="7"/>
       <c r="L352" s="7"/>
@@ -17380,15 +17391,15 @@
       <c r="S352" s="7"/>
     </row>
     <row r="353" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="94"/>
+      <c r="A353" s="93"/>
       <c r="B353" s="7"/>
-      <c r="C353" s="95"/>
-      <c r="D353" s="95"/>
-      <c r="E353" s="94"/>
-      <c r="F353" s="94"/>
-      <c r="G353" s="94"/>
-      <c r="H353" s="96"/>
-      <c r="I353" s="94"/>
+      <c r="C353" s="94"/>
+      <c r="D353" s="94"/>
+      <c r="E353" s="93"/>
+      <c r="F353" s="93"/>
+      <c r="G353" s="93"/>
+      <c r="H353" s="95"/>
+      <c r="I353" s="93"/>
       <c r="J353" s="7"/>
       <c r="K353" s="7"/>
       <c r="L353" s="7"/>
@@ -17401,15 +17412,15 @@
       <c r="S353" s="7"/>
     </row>
     <row r="354" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="94"/>
+      <c r="A354" s="93"/>
       <c r="B354" s="7"/>
-      <c r="C354" s="95"/>
-      <c r="D354" s="95"/>
-      <c r="E354" s="94"/>
-      <c r="F354" s="94"/>
-      <c r="G354" s="94"/>
-      <c r="H354" s="96"/>
-      <c r="I354" s="94"/>
+      <c r="C354" s="94"/>
+      <c r="D354" s="94"/>
+      <c r="E354" s="93"/>
+      <c r="F354" s="93"/>
+      <c r="G354" s="93"/>
+      <c r="H354" s="95"/>
+      <c r="I354" s="93"/>
       <c r="J354" s="7"/>
       <c r="K354" s="7"/>
       <c r="L354" s="7"/>
@@ -17422,15 +17433,15 @@
       <c r="S354" s="7"/>
     </row>
     <row r="355" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="94"/>
+      <c r="A355" s="93"/>
       <c r="B355" s="7"/>
-      <c r="C355" s="95"/>
-      <c r="D355" s="95"/>
-      <c r="E355" s="94"/>
-      <c r="F355" s="94"/>
-      <c r="G355" s="94"/>
-      <c r="H355" s="96"/>
-      <c r="I355" s="94"/>
+      <c r="C355" s="94"/>
+      <c r="D355" s="94"/>
+      <c r="E355" s="93"/>
+      <c r="F355" s="93"/>
+      <c r="G355" s="93"/>
+      <c r="H355" s="95"/>
+      <c r="I355" s="93"/>
       <c r="J355" s="7"/>
       <c r="K355" s="7"/>
       <c r="L355" s="7"/>
@@ -17443,15 +17454,15 @@
       <c r="S355" s="7"/>
     </row>
     <row r="356" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="94"/>
+      <c r="A356" s="93"/>
       <c r="B356" s="7"/>
-      <c r="C356" s="95"/>
-      <c r="D356" s="95"/>
-      <c r="E356" s="94"/>
-      <c r="F356" s="94"/>
-      <c r="G356" s="94"/>
-      <c r="H356" s="96"/>
-      <c r="I356" s="94"/>
+      <c r="C356" s="94"/>
+      <c r="D356" s="94"/>
+      <c r="E356" s="93"/>
+      <c r="F356" s="93"/>
+      <c r="G356" s="93"/>
+      <c r="H356" s="95"/>
+      <c r="I356" s="93"/>
       <c r="J356" s="7"/>
       <c r="K356" s="7"/>
       <c r="L356" s="7"/>
@@ -17464,15 +17475,15 @@
       <c r="S356" s="7"/>
     </row>
     <row r="357" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="94"/>
+      <c r="A357" s="93"/>
       <c r="B357" s="7"/>
-      <c r="C357" s="95"/>
-      <c r="D357" s="95"/>
-      <c r="E357" s="94"/>
-      <c r="F357" s="94"/>
-      <c r="G357" s="94"/>
-      <c r="H357" s="96"/>
-      <c r="I357" s="94"/>
+      <c r="C357" s="94"/>
+      <c r="D357" s="94"/>
+      <c r="E357" s="93"/>
+      <c r="F357" s="93"/>
+      <c r="G357" s="93"/>
+      <c r="H357" s="95"/>
+      <c r="I357" s="93"/>
       <c r="J357" s="7"/>
       <c r="K357" s="7"/>
       <c r="L357" s="7"/>
@@ -17485,15 +17496,15 @@
       <c r="S357" s="7"/>
     </row>
     <row r="358" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="94"/>
+      <c r="A358" s="93"/>
       <c r="B358" s="7"/>
-      <c r="C358" s="95"/>
-      <c r="D358" s="95"/>
-      <c r="E358" s="94"/>
-      <c r="F358" s="94"/>
-      <c r="G358" s="94"/>
-      <c r="H358" s="96"/>
-      <c r="I358" s="94"/>
+      <c r="C358" s="94"/>
+      <c r="D358" s="94"/>
+      <c r="E358" s="93"/>
+      <c r="F358" s="93"/>
+      <c r="G358" s="93"/>
+      <c r="H358" s="95"/>
+      <c r="I358" s="93"/>
       <c r="J358" s="7"/>
       <c r="K358" s="7"/>
       <c r="L358" s="7"/>
@@ -17506,15 +17517,15 @@
       <c r="S358" s="7"/>
     </row>
     <row r="359" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="94"/>
+      <c r="A359" s="93"/>
       <c r="B359" s="7"/>
-      <c r="C359" s="95"/>
-      <c r="D359" s="95"/>
-      <c r="E359" s="94"/>
-      <c r="F359" s="94"/>
-      <c r="G359" s="94"/>
-      <c r="H359" s="96"/>
-      <c r="I359" s="94"/>
+      <c r="C359" s="94"/>
+      <c r="D359" s="94"/>
+      <c r="E359" s="93"/>
+      <c r="F359" s="93"/>
+      <c r="G359" s="93"/>
+      <c r="H359" s="95"/>
+      <c r="I359" s="93"/>
       <c r="J359" s="7"/>
       <c r="K359" s="7"/>
       <c r="L359" s="7"/>
@@ -17527,15 +17538,15 @@
       <c r="S359" s="7"/>
     </row>
     <row r="360" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="94"/>
+      <c r="A360" s="93"/>
       <c r="B360" s="7"/>
-      <c r="C360" s="95"/>
-      <c r="D360" s="95"/>
-      <c r="E360" s="94"/>
-      <c r="F360" s="94"/>
-      <c r="G360" s="94"/>
-      <c r="H360" s="96"/>
-      <c r="I360" s="94"/>
+      <c r="C360" s="94"/>
+      <c r="D360" s="94"/>
+      <c r="E360" s="93"/>
+      <c r="F360" s="93"/>
+      <c r="G360" s="93"/>
+      <c r="H360" s="95"/>
+      <c r="I360" s="93"/>
       <c r="J360" s="7"/>
       <c r="K360" s="7"/>
       <c r="L360" s="7"/>
@@ -17548,15 +17559,15 @@
       <c r="S360" s="7"/>
     </row>
     <row r="361" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="94"/>
+      <c r="A361" s="93"/>
       <c r="B361" s="7"/>
-      <c r="C361" s="95"/>
-      <c r="D361" s="95"/>
-      <c r="E361" s="94"/>
-      <c r="F361" s="94"/>
-      <c r="G361" s="94"/>
-      <c r="H361" s="96"/>
-      <c r="I361" s="94"/>
+      <c r="C361" s="94"/>
+      <c r="D361" s="94"/>
+      <c r="E361" s="93"/>
+      <c r="F361" s="93"/>
+      <c r="G361" s="93"/>
+      <c r="H361" s="95"/>
+      <c r="I361" s="93"/>
       <c r="J361" s="7"/>
       <c r="K361" s="7"/>
       <c r="L361" s="7"/>
@@ -17569,15 +17580,15 @@
       <c r="S361" s="7"/>
     </row>
     <row r="362" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="94"/>
+      <c r="A362" s="93"/>
       <c r="B362" s="7"/>
-      <c r="C362" s="95"/>
-      <c r="D362" s="95"/>
-      <c r="E362" s="94"/>
-      <c r="F362" s="94"/>
-      <c r="G362" s="94"/>
-      <c r="H362" s="96"/>
-      <c r="I362" s="94"/>
+      <c r="C362" s="94"/>
+      <c r="D362" s="94"/>
+      <c r="E362" s="93"/>
+      <c r="F362" s="93"/>
+      <c r="G362" s="93"/>
+      <c r="H362" s="95"/>
+      <c r="I362" s="93"/>
       <c r="J362" s="7"/>
       <c r="K362" s="7"/>
       <c r="L362" s="7"/>
@@ -17660,16 +17671,16 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="97" width="6.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="97" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="97" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="97" width="36.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="97" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="96" width="6.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="96" width="17.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="96" width="40.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="96" width="36.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="96" width="7.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17716,28 +17727,28 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
@@ -17775,19 +17786,19 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="98" t="s">
         <v>1003</v>
       </c>
-      <c r="B7" s="99"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="n">
@@ -17796,7 +17807,7 @@
       <c r="B8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="100" t="s">
+      <c r="C8" s="99" t="s">
         <v>1004</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -17832,7 +17843,7 @@
       <c r="B9" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="100" t="s">
         <v>1006</v>
       </c>
       <c r="D9" s="25" t="s">
@@ -17868,7 +17879,7 @@
       <c r="B10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="100" t="s">
+      <c r="C10" s="99" t="s">
         <v>1008</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -17904,10 +17915,10 @@
       <c r="B11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="102" t="s">
+      <c r="C11" s="101" t="s">
         <v>1010</v>
       </c>
-      <c r="D11" s="103" t="s">
+      <c r="D11" s="102" t="s">
         <v>1011</v>
       </c>
       <c r="E11" s="24" t="s">
@@ -17916,7 +17927,7 @@
       <c r="F11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="104" t="s">
+      <c r="G11" s="103" t="s">
         <v>997</v>
       </c>
       <c r="H11" s="21" t="s">
@@ -17925,7 +17936,7 @@
       <c r="I11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="103" t="s">
+      <c r="J11" s="102" t="s">
         <v>1011</v>
       </c>
       <c r="K11" s="19" t="s">
@@ -17940,10 +17951,10 @@
       <c r="B12" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="102" t="s">
+      <c r="C12" s="101" t="s">
         <v>1012</v>
       </c>
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="102" t="s">
         <v>1013</v>
       </c>
       <c r="E12" s="24" t="s">
@@ -17952,7 +17963,7 @@
       <c r="F12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="104" t="s">
+      <c r="G12" s="103" t="s">
         <v>711</v>
       </c>
       <c r="H12" s="21" t="s">
@@ -17961,7 +17972,7 @@
       <c r="I12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="103" t="s">
+      <c r="J12" s="102" t="s">
         <v>1013</v>
       </c>
       <c r="K12" s="19" t="s">
@@ -17976,10 +17987,10 @@
       <c r="B13" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="C13" s="101" t="s">
         <v>1014</v>
       </c>
-      <c r="D13" s="103" t="s">
+      <c r="D13" s="102" t="s">
         <v>1015</v>
       </c>
       <c r="E13" s="24" t="s">
@@ -17988,7 +17999,7 @@
       <c r="F13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="104" t="s">
+      <c r="G13" s="103" t="s">
         <v>267</v>
       </c>
       <c r="H13" s="21" t="s">
@@ -17997,7 +18008,7 @@
       <c r="I13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="103" t="s">
+      <c r="J13" s="102" t="s">
         <v>1015</v>
       </c>
       <c r="K13" s="19" t="s">
@@ -18012,10 +18023,10 @@
       <c r="B14" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="102" t="s">
+      <c r="C14" s="101" t="s">
         <v>1016</v>
       </c>
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="102" t="s">
         <v>1017</v>
       </c>
       <c r="E14" s="24" t="s">
@@ -18024,7 +18035,7 @@
       <c r="F14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="104" t="s">
+      <c r="G14" s="103" t="s">
         <v>61</v>
       </c>
       <c r="H14" s="21" t="s">
@@ -18033,7 +18044,7 @@
       <c r="I14" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="103" t="s">
+      <c r="J14" s="102" t="s">
         <v>1017</v>
       </c>
       <c r="K14" s="19" t="s">
@@ -18048,10 +18059,10 @@
       <c r="B15" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="102" t="s">
+      <c r="C15" s="101" t="s">
         <v>1018</v>
       </c>
-      <c r="D15" s="103" t="s">
+      <c r="D15" s="102" t="s">
         <v>1019</v>
       </c>
       <c r="E15" s="24" t="s">
@@ -18060,7 +18071,7 @@
       <c r="F15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="104" t="s">
+      <c r="G15" s="103" t="s">
         <v>375</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -18069,7 +18080,7 @@
       <c r="I15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="102" t="s">
         <v>1020</v>
       </c>
       <c r="K15" s="19" t="s">
@@ -18084,10 +18095,10 @@
       <c r="B16" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="102" t="s">
+      <c r="C16" s="101" t="s">
         <v>1021</v>
       </c>
-      <c r="D16" s="103" t="s">
+      <c r="D16" s="102" t="s">
         <v>1022</v>
       </c>
       <c r="E16" s="24" t="s">
@@ -18096,7 +18107,7 @@
       <c r="F16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="104" t="s">
+      <c r="G16" s="103" t="s">
         <v>1023</v>
       </c>
       <c r="H16" s="21" t="s">
@@ -18105,7 +18116,7 @@
       <c r="I16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="103" t="s">
+      <c r="J16" s="102" t="s">
         <v>1024</v>
       </c>
       <c r="K16" s="19" t="s">
@@ -18120,10 +18131,10 @@
       <c r="B17" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="102" t="s">
+      <c r="C17" s="101" t="s">
         <v>1025</v>
       </c>
-      <c r="D17" s="103" t="s">
+      <c r="D17" s="102" t="s">
         <v>1026</v>
       </c>
       <c r="E17" s="24" t="s">
@@ -18132,7 +18143,7 @@
       <c r="F17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="104" t="s">
+      <c r="G17" s="103" t="s">
         <v>1027</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -18141,7 +18152,7 @@
       <c r="I17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="103" t="s">
+      <c r="J17" s="102" t="s">
         <v>1028</v>
       </c>
       <c r="K17" s="19" t="s">
@@ -18156,10 +18167,10 @@
       <c r="B18" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="102" t="s">
+      <c r="C18" s="101" t="s">
         <v>1029</v>
       </c>
-      <c r="D18" s="103" t="s">
+      <c r="D18" s="102" t="s">
         <v>1030</v>
       </c>
       <c r="E18" s="24" t="s">
@@ -18168,7 +18179,7 @@
       <c r="F18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="104" t="s">
+      <c r="G18" s="103" t="s">
         <v>1027</v>
       </c>
       <c r="H18" s="21" t="s">
@@ -18177,14 +18188,14 @@
       <c r="I18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="103" t="s">
+      <c r="J18" s="102" t="s">
         <v>1031</v>
       </c>
       <c r="K18" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="n">
         <f aca="false">A18+1</f>
         <v>12</v>
@@ -18192,10 +18203,10 @@
       <c r="B19" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="101" t="s">
         <v>1032</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="102" t="s">
         <v>1033</v>
       </c>
       <c r="E19" s="24" t="s">
@@ -18213,7 +18224,7 @@
       <c r="I19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="103" t="s">
+      <c r="J19" s="102" t="s">
         <v>1034</v>
       </c>
       <c r="K19" s="19" t="s">
@@ -18228,10 +18239,10 @@
       <c r="B20" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="102" t="s">
+      <c r="C20" s="101" t="s">
         <v>1035</v>
       </c>
-      <c r="D20" s="103" t="s">
+      <c r="D20" s="102" t="s">
         <v>1036</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -18240,8 +18251,8 @@
       <c r="F20" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="104" t="s">
-        <v>1027</v>
+      <c r="G20" s="103" t="s">
+        <v>1037</v>
       </c>
       <c r="H20" s="21" t="s">
         <v>17</v>
@@ -18249,7 +18260,7 @@
       <c r="I20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="103" t="s">
+      <c r="J20" s="102" t="s">
         <v>1036</v>
       </c>
       <c r="K20" s="19" t="s">
@@ -18264,11 +18275,11 @@
       <c r="B21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="102" t="s">
-        <v>1037</v>
-      </c>
-      <c r="D21" s="103" t="s">
+      <c r="C21" s="101" t="s">
         <v>1038</v>
+      </c>
+      <c r="D21" s="102" t="s">
+        <v>1039</v>
       </c>
       <c r="E21" s="24" t="s">
         <v>23</v>
@@ -18276,8 +18287,8 @@
       <c r="F21" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="104" t="s">
-        <v>1027</v>
+      <c r="G21" s="103" t="s">
+        <v>1040</v>
       </c>
       <c r="H21" s="21" t="s">
         <v>17</v>
@@ -18285,8 +18296,8 @@
       <c r="I21" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="103" t="s">
-        <v>1038</v>
+      <c r="J21" s="102" t="s">
+        <v>1039</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>20</v>
@@ -18300,11 +18311,11 @@
       <c r="B22" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="102" t="s">
-        <v>1039</v>
-      </c>
-      <c r="D22" s="103" t="s">
-        <v>1040</v>
+      <c r="C22" s="101" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D22" s="102" t="s">
+        <v>1042</v>
       </c>
       <c r="E22" s="24" t="s">
         <v>23</v>
@@ -18312,8 +18323,8 @@
       <c r="F22" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="104" t="s">
-        <v>1041</v>
+      <c r="G22" s="103" t="s">
+        <v>1043</v>
       </c>
       <c r="H22" s="21" t="s">
         <v>17</v>
@@ -18321,8 +18332,8 @@
       <c r="I22" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="103" t="s">
-        <v>1042</v>
+      <c r="J22" s="102" t="s">
+        <v>1044</v>
       </c>
       <c r="K22" s="19" t="s">
         <v>20</v>
@@ -18336,11 +18347,11 @@
       <c r="B23" s="105" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="102" t="s">
-        <v>1043</v>
-      </c>
-      <c r="D23" s="103" t="s">
-        <v>1044</v>
+      <c r="C23" s="101" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D23" s="102" t="s">
+        <v>1046</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>15</v>
@@ -18348,7 +18359,7 @@
       <c r="F23" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="104" t="s">
+      <c r="G23" s="103" t="s">
         <v>17</v>
       </c>
       <c r="H23" s="21" t="s">
@@ -18357,8 +18368,8 @@
       <c r="I23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="103" t="s">
-        <v>1044</v>
+      <c r="J23" s="102" t="s">
+        <v>1046</v>
       </c>
       <c r="K23" s="19" t="s">
         <v>20</v>
@@ -18372,19 +18383,19 @@
       <c r="B24" s="105" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="102" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D24" s="103" t="s">
-        <v>1046</v>
+      <c r="C24" s="101" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D24" s="102" t="s">
+        <v>1048</v>
       </c>
       <c r="E24" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="104" t="s">
+      <c r="F24" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="104" t="s">
+      <c r="G24" s="103" t="s">
         <v>56</v>
       </c>
       <c r="H24" s="21" t="s">
@@ -18393,8 +18404,8 @@
       <c r="I24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="103" t="s">
-        <v>1046</v>
+      <c r="J24" s="102" t="s">
+        <v>1048</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>20</v>
@@ -18408,20 +18419,20 @@
       <c r="B25" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="102" t="s">
-        <v>1047</v>
-      </c>
-      <c r="D25" s="103" t="s">
-        <v>1048</v>
+      <c r="C25" s="101" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D25" s="102" t="s">
+        <v>1050</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="104" t="s">
+      <c r="F25" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="G25" s="104" t="s">
-        <v>1049</v>
+      <c r="G25" s="103" t="s">
+        <v>1051</v>
       </c>
       <c r="H25" s="21" t="s">
         <v>17</v>
@@ -18429,8 +18440,8 @@
       <c r="I25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="103" t="s">
-        <v>1048</v>
+      <c r="J25" s="102" t="s">
+        <v>1050</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>20</v>
@@ -18445,10 +18456,10 @@
         <v>143</v>
       </c>
       <c r="C26" s="107" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="D26" s="108" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>15</v>
@@ -18466,7 +18477,7 @@
         <v>17</v>
       </c>
       <c r="J26" s="108" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="K26" s="30" t="s">
         <v>20</v>
@@ -18481,10 +18492,10 @@
         <v>146</v>
       </c>
       <c r="C27" s="110" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="D27" s="111" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E27" s="112" t="s">
         <v>23</v>
@@ -18493,7 +18504,7 @@
         <v>143</v>
       </c>
       <c r="G27" s="112" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="H27" s="112" t="s">
         <v>17</v>
@@ -18502,7 +18513,7 @@
         <v>17</v>
       </c>
       <c r="J27" s="111" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="K27" s="30" t="s">
         <v>20</v>
@@ -18517,10 +18528,10 @@
         <v>150</v>
       </c>
       <c r="C28" s="110" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="D28" s="111" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E28" s="112" t="s">
         <v>23</v>
@@ -18529,7 +18540,7 @@
         <v>143</v>
       </c>
       <c r="G28" s="112" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="H28" s="112" t="s">
         <v>17</v>
@@ -18538,7 +18549,7 @@
         <v>17</v>
       </c>
       <c r="J28" s="111" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="K28" s="30" t="s">
         <v>20</v>

</xml_diff>